<commit_message>
Refactoring the OngyAi app
</commit_message>
<xml_diff>
--- a/data_fetching/Entsoe/Actual_Production_Hydro_River.xlsx
+++ b/data_fetching/Entsoe/Actual_Production_Hydro_River.xlsx
@@ -381,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B289"/>
+  <dimension ref="A1:B385"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -397,2305 +397,3073 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>45685</v>
+        <v>45730</v>
       </c>
       <c r="B2">
-        <v>610</v>
+        <v>642</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>45685.01041666666</v>
+        <v>45730.01041666666</v>
       </c>
       <c r="B3">
-        <v>603</v>
+        <v>634</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>45685.02083333334</v>
+        <v>45730.02083333334</v>
       </c>
       <c r="B4">
-        <v>604</v>
+        <v>631</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>45685.03125</v>
+        <v>45730.03125</v>
       </c>
       <c r="B5">
-        <v>603</v>
+        <v>631</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>45685.04166666666</v>
+        <v>45730.04166666666</v>
       </c>
       <c r="B6">
-        <v>603</v>
+        <v>613</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>45685.05208333334</v>
+        <v>45730.05208333334</v>
       </c>
       <c r="B7">
-        <v>603</v>
+        <v>613</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>45685.0625</v>
+        <v>45730.0625</v>
       </c>
       <c r="B8">
-        <v>604</v>
+        <v>613</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>45685.07291666666</v>
+        <v>45730.07291666666</v>
       </c>
       <c r="B9">
-        <v>604</v>
+        <v>612</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>45685.08333333334</v>
+        <v>45730.08333333334</v>
       </c>
       <c r="B10">
-        <v>605</v>
+        <v>618</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>45685.09375</v>
+        <v>45730.09375</v>
       </c>
       <c r="B11">
-        <v>604</v>
+        <v>615</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>45685.10416666666</v>
+        <v>45730.10416666666</v>
       </c>
       <c r="B12">
-        <v>604</v>
+        <v>614</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>45685.11458333334</v>
+        <v>45730.11458333334</v>
       </c>
       <c r="B13">
-        <v>604</v>
+        <v>615</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>45685.125</v>
+        <v>45730.125</v>
       </c>
       <c r="B14">
-        <v>604</v>
+        <v>642</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>45685.13541666666</v>
+        <v>45730.13541666666</v>
       </c>
       <c r="B15">
-        <v>603</v>
+        <v>644</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>45685.14583333334</v>
+        <v>45730.14583333334</v>
       </c>
       <c r="B16">
-        <v>603</v>
+        <v>668</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>45685.15625</v>
+        <v>45730.15625</v>
       </c>
       <c r="B17">
-        <v>603</v>
+        <v>693</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>45685.16666666666</v>
+        <v>45730.16666666666</v>
       </c>
       <c r="B18">
-        <v>603</v>
+        <v>843</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>45685.17708333334</v>
+        <v>45730.17708333334</v>
       </c>
       <c r="B19">
-        <v>604</v>
+        <v>848</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>45685.1875</v>
+        <v>45730.1875</v>
       </c>
       <c r="B20">
-        <v>603</v>
+        <v>849</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>45685.19791666666</v>
+        <v>45730.19791666666</v>
       </c>
       <c r="B21">
-        <v>605</v>
+        <v>830</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>45685.20833333334</v>
+        <v>45730.20833333334</v>
       </c>
       <c r="B22">
-        <v>665</v>
+        <v>821</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>45685.21875</v>
+        <v>45730.21875</v>
       </c>
       <c r="B23">
-        <v>674</v>
+        <v>803</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>45685.22916666666</v>
+        <v>45730.22916666666</v>
       </c>
       <c r="B24">
-        <v>675</v>
+        <v>802</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>45685.23958333334</v>
+        <v>45730.23958333334</v>
       </c>
       <c r="B25">
-        <v>677</v>
+        <v>803</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>45685.25</v>
+        <v>45730.25</v>
       </c>
       <c r="B26">
-        <v>803</v>
+        <v>901</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
-        <v>45685.26041666666</v>
+        <v>45730.26041666666</v>
       </c>
       <c r="B27">
-        <v>828</v>
+        <v>921</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
-        <v>45685.27083333334</v>
+        <v>45730.27083333334</v>
       </c>
       <c r="B28">
-        <v>828</v>
+        <v>869</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
-        <v>45685.28125</v>
+        <v>45730.28125</v>
       </c>
       <c r="B29">
-        <v>829</v>
+        <v>840</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2">
-        <v>45685.29166666666</v>
+        <v>45730.29166666666</v>
       </c>
       <c r="B30">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2">
-        <v>45685.30208333334</v>
+        <v>45730.30208333334</v>
       </c>
       <c r="B31">
-        <v>872</v>
+        <v>862</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2">
-        <v>45685.3125</v>
+        <v>45730.3125</v>
       </c>
       <c r="B32">
-        <v>872</v>
+        <v>933</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2">
-        <v>45685.32291666666</v>
+        <v>45730.32291666666</v>
       </c>
       <c r="B33">
-        <v>876</v>
+        <v>941</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2">
-        <v>45685.33333333334</v>
+        <v>45730.33333333334</v>
       </c>
       <c r="B34">
-        <v>952</v>
+        <v>827</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2">
-        <v>45685.34375</v>
+        <v>45730.34375</v>
       </c>
       <c r="B35">
-        <v>958</v>
+        <v>819</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2">
-        <v>45685.35416666666</v>
+        <v>45730.35416666666</v>
       </c>
       <c r="B36">
-        <v>959</v>
+        <v>815</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2">
-        <v>45685.36458333334</v>
+        <v>45730.36458333334</v>
       </c>
       <c r="B37">
-        <v>932</v>
+        <v>812</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2">
-        <v>45685.375</v>
+        <v>45730.375</v>
       </c>
       <c r="B38">
-        <v>905</v>
+        <v>820</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2">
-        <v>45685.38541666666</v>
+        <v>45730.38541666666</v>
       </c>
       <c r="B39">
-        <v>902</v>
+        <v>841</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2">
-        <v>45685.39583333334</v>
+        <v>45730.39583333334</v>
       </c>
       <c r="B40">
-        <v>892</v>
+        <v>849</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2">
-        <v>45685.40625</v>
+        <v>45730.40625</v>
       </c>
       <c r="B41">
-        <v>890</v>
+        <v>851</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2">
-        <v>45685.41666666666</v>
+        <v>45730.41666666666</v>
       </c>
       <c r="B42">
-        <v>866</v>
+        <v>828</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2">
-        <v>45685.42708333334</v>
+        <v>45730.42708333334</v>
       </c>
       <c r="B43">
-        <v>865</v>
+        <v>825</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2">
-        <v>45685.4375</v>
+        <v>45730.4375</v>
       </c>
       <c r="B44">
-        <v>863</v>
+        <v>784</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2">
-        <v>45685.44791666666</v>
+        <v>45730.44791666666</v>
       </c>
       <c r="B45">
-        <v>857</v>
+        <v>727</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2">
-        <v>45685.45833333334</v>
+        <v>45730.45833333334</v>
       </c>
       <c r="B46">
-        <v>714</v>
+        <v>565</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2">
-        <v>45685.46875</v>
+        <v>45730.46875</v>
       </c>
       <c r="B47">
-        <v>707</v>
+        <v>558</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2">
-        <v>45685.47916666666</v>
+        <v>45730.47916666666</v>
       </c>
       <c r="B48">
-        <v>770</v>
+        <v>580</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2">
-        <v>45685.48958333334</v>
+        <v>45730.48958333334</v>
       </c>
       <c r="B49">
-        <v>776</v>
+        <v>587</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2">
-        <v>45685.5</v>
+        <v>45730.5</v>
       </c>
       <c r="B50">
-        <v>786</v>
+        <v>579</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2">
-        <v>45685.51041666666</v>
+        <v>45730.51041666666</v>
       </c>
       <c r="B51">
-        <v>786</v>
+        <v>577</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2">
-        <v>45685.52083333334</v>
+        <v>45730.52083333334</v>
       </c>
       <c r="B52">
-        <v>786</v>
+        <v>578</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2">
-        <v>45685.53125</v>
+        <v>45730.53125</v>
       </c>
       <c r="B53">
-        <v>786</v>
+        <v>581</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2">
-        <v>45685.54166666666</v>
+        <v>45730.54166666666</v>
       </c>
       <c r="B54">
-        <v>777</v>
+        <v>588</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2">
-        <v>45685.55208333334</v>
+        <v>45730.55208333334</v>
       </c>
       <c r="B55">
-        <v>757</v>
+        <v>592</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2">
-        <v>45685.5625</v>
+        <v>45730.5625</v>
       </c>
       <c r="B56">
-        <v>757</v>
+        <v>631</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2">
-        <v>45685.57291666666</v>
+        <v>45730.57291666666</v>
       </c>
       <c r="B57">
-        <v>757</v>
+        <v>664</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2">
-        <v>45685.58333333334</v>
+        <v>45730.58333333334</v>
       </c>
       <c r="B58">
-        <v>713</v>
+        <v>749</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2">
-        <v>45685.59375</v>
+        <v>45730.59375</v>
       </c>
       <c r="B59">
-        <v>711</v>
+        <v>699</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2">
-        <v>45685.60416666666</v>
+        <v>45730.60416666666</v>
       </c>
       <c r="B60">
-        <v>712</v>
+        <v>696</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2">
-        <v>45685.61458333334</v>
+        <v>45730.61458333334</v>
       </c>
       <c r="B61">
-        <v>694</v>
+        <v>701</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2">
-        <v>45685.625</v>
+        <v>45730.625</v>
       </c>
       <c r="B62">
-        <v>700</v>
+        <v>808</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2">
-        <v>45685.63541666666</v>
+        <v>45730.63541666666</v>
       </c>
       <c r="B63">
-        <v>701</v>
+        <v>834</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2">
-        <v>45685.64583333334</v>
+        <v>45730.64583333334</v>
       </c>
       <c r="B64">
-        <v>702</v>
+        <v>836</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2">
-        <v>45685.65625</v>
+        <v>45730.65625</v>
       </c>
       <c r="B65">
-        <v>766</v>
+        <v>837</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2">
-        <v>45685.66666666666</v>
+        <v>45730.66666666666</v>
       </c>
       <c r="B66">
-        <v>781</v>
+        <v>839</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2">
-        <v>45685.67708333334</v>
+        <v>45730.67708333334</v>
       </c>
       <c r="B67">
-        <v>784</v>
+        <v>839</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2">
-        <v>45685.6875</v>
+        <v>45730.6875</v>
       </c>
       <c r="B68">
-        <v>784</v>
+        <v>840</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2">
-        <v>45685.69791666666</v>
+        <v>45730.69791666666</v>
       </c>
       <c r="B69">
-        <v>786</v>
+        <v>850</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2">
-        <v>45685.70833333334</v>
+        <v>45730.70833333334</v>
       </c>
       <c r="B70">
-        <v>966</v>
+        <v>930</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2">
-        <v>45685.71875</v>
+        <v>45730.71875</v>
       </c>
       <c r="B71">
-        <v>990</v>
+        <v>932</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="2">
-        <v>45685.72916666666</v>
+        <v>45730.72916666666</v>
       </c>
       <c r="B72">
-        <v>989</v>
+        <v>932</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2">
-        <v>45685.73958333334</v>
+        <v>45730.73958333334</v>
       </c>
       <c r="B73">
-        <v>990</v>
+        <v>932</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="2">
-        <v>45685.75</v>
+        <v>45730.75</v>
       </c>
       <c r="B74">
-        <v>996</v>
+        <v>917</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="2">
-        <v>45685.76041666666</v>
+        <v>45730.76041666666</v>
       </c>
       <c r="B75">
-        <v>996</v>
+        <v>924</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="2">
-        <v>45685.77083333334</v>
+        <v>45730.77083333334</v>
       </c>
       <c r="B76">
-        <v>996</v>
+        <v>923</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="2">
-        <v>45685.78125</v>
+        <v>45730.78125</v>
       </c>
       <c r="B77">
-        <v>997</v>
+        <v>924</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="2">
-        <v>45685.79166666666</v>
+        <v>45730.79166666666</v>
       </c>
       <c r="B78">
-        <v>1011</v>
+        <v>930</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="2">
-        <v>45685.80208333334</v>
+        <v>45730.80208333334</v>
       </c>
       <c r="B79">
-        <v>1009</v>
+        <v>928</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="2">
-        <v>45685.8125</v>
+        <v>45730.8125</v>
       </c>
       <c r="B80">
-        <v>1008</v>
+        <v>928</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="2">
-        <v>45685.82291666666</v>
+        <v>45730.82291666666</v>
       </c>
       <c r="B81">
-        <v>1008</v>
+        <v>928</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="2">
-        <v>45685.83333333334</v>
+        <v>45730.83333333334</v>
       </c>
       <c r="B82">
-        <v>1003</v>
+        <v>917</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="2">
-        <v>45685.84375</v>
+        <v>45730.84375</v>
       </c>
       <c r="B83">
-        <v>998</v>
+        <v>909</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="2">
-        <v>45685.85416666666</v>
+        <v>45730.85416666666</v>
       </c>
       <c r="B84">
-        <v>998</v>
+        <v>910</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="2">
-        <v>45685.86458333334</v>
+        <v>45730.86458333334</v>
       </c>
       <c r="B85">
-        <v>998</v>
+        <v>906</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="2">
-        <v>45685.875</v>
+        <v>45730.875</v>
       </c>
       <c r="B86">
-        <v>1014</v>
+        <v>922</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="2">
-        <v>45685.88541666666</v>
+        <v>45730.88541666666</v>
       </c>
       <c r="B87">
-        <v>1017</v>
+        <v>919</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="2">
-        <v>45685.89583333334</v>
+        <v>45730.89583333334</v>
       </c>
       <c r="B88">
-        <v>1016</v>
+        <v>924</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="2">
-        <v>45685.90625</v>
+        <v>45730.90625</v>
       </c>
       <c r="B89">
-        <v>1015</v>
+        <v>922</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="2">
-        <v>45685.91666666666</v>
+        <v>45730.91666666666</v>
       </c>
       <c r="B90">
-        <v>832</v>
+        <v>770</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="2">
-        <v>45685.92708333334</v>
+        <v>45730.92708333334</v>
       </c>
       <c r="B91">
-        <v>820</v>
+        <v>747</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="2">
-        <v>45685.9375</v>
+        <v>45730.9375</v>
       </c>
       <c r="B92">
-        <v>821</v>
+        <v>747</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="2">
-        <v>45685.94791666666</v>
+        <v>45730.94791666666</v>
       </c>
       <c r="B93">
-        <v>818</v>
+        <v>748</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="2">
-        <v>45685.95833333334</v>
+        <v>45730.95833333334</v>
       </c>
       <c r="B94">
-        <v>608</v>
+        <v>773</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="2">
-        <v>45685.96875</v>
+        <v>45730.96875</v>
       </c>
       <c r="B95">
-        <v>602</v>
+        <v>772</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="2">
-        <v>45685.97916666666</v>
+        <v>45730.97916666666</v>
       </c>
       <c r="B96">
-        <v>602</v>
+        <v>777</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="2">
-        <v>45685.98958333334</v>
+        <v>45730.98958333334</v>
       </c>
       <c r="B97">
-        <v>602</v>
+        <v>777</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="2">
-        <v>45686</v>
+        <v>45731</v>
       </c>
       <c r="B98">
-        <v>577</v>
+        <v>744</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="2">
-        <v>45686.01041666666</v>
+        <v>45731.01041666666</v>
       </c>
       <c r="B99">
-        <v>574</v>
+        <v>748</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="2">
-        <v>45686.02083333334</v>
+        <v>45731.02083333334</v>
       </c>
       <c r="B100">
-        <v>575</v>
+        <v>782</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="2">
-        <v>45686.03125</v>
+        <v>45731.03125</v>
       </c>
       <c r="B101">
-        <v>575</v>
+        <v>782</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="2">
-        <v>45686.04166666666</v>
+        <v>45731.04166666666</v>
       </c>
       <c r="B102">
-        <v>575</v>
+        <v>753</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="2">
-        <v>45686.05208333334</v>
+        <v>45731.05208333334</v>
       </c>
       <c r="B103">
-        <v>575</v>
+        <v>752</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="2">
-        <v>45686.0625</v>
+        <v>45731.0625</v>
       </c>
       <c r="B104">
-        <v>575</v>
+        <v>752</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="2">
-        <v>45686.07291666666</v>
+        <v>45731.07291666666</v>
       </c>
       <c r="B105">
-        <v>575</v>
+        <v>752</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="2">
-        <v>45686.08333333334</v>
+        <v>45731.08333333334</v>
       </c>
       <c r="B106">
-        <v>577</v>
+        <v>761</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="2">
-        <v>45686.09375</v>
+        <v>45731.09375</v>
       </c>
       <c r="B107">
-        <v>575</v>
+        <v>753</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="2">
-        <v>45686.10416666666</v>
+        <v>45731.10416666666</v>
       </c>
       <c r="B108">
-        <v>575</v>
+        <v>753</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="2">
-        <v>45686.11458333334</v>
+        <v>45731.11458333334</v>
       </c>
       <c r="B109">
-        <v>575</v>
+        <v>756</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="2">
-        <v>45686.125</v>
+        <v>45731.125</v>
       </c>
       <c r="B110">
-        <v>575</v>
+        <v>828</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="2">
-        <v>45686.13541666666</v>
+        <v>45731.13541666666</v>
       </c>
       <c r="B111">
-        <v>575</v>
+        <v>830</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="2">
-        <v>45686.14583333334</v>
+        <v>45731.14583333334</v>
       </c>
       <c r="B112">
-        <v>575</v>
+        <v>831</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="2">
-        <v>45686.15625</v>
+        <v>45731.15625</v>
       </c>
       <c r="B113">
-        <v>575</v>
+        <v>832</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="2">
-        <v>45686.16666666666</v>
+        <v>45731.16666666666</v>
       </c>
       <c r="B114">
-        <v>589</v>
+        <v>842</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="2">
-        <v>45686.17708333334</v>
+        <v>45731.17708333334</v>
       </c>
       <c r="B115">
-        <v>590</v>
+        <v>843</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="2">
-        <v>45686.1875</v>
+        <v>45731.1875</v>
       </c>
       <c r="B116">
-        <v>591</v>
+        <v>843</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="2">
-        <v>45686.19791666666</v>
+        <v>45731.19791666666</v>
       </c>
       <c r="B117">
-        <v>597</v>
+        <v>842</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="2">
-        <v>45686.20833333334</v>
+        <v>45731.20833333334</v>
       </c>
       <c r="B118">
-        <v>692</v>
+        <v>821</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="2">
-        <v>45686.21875</v>
+        <v>45731.21875</v>
       </c>
       <c r="B119">
-        <v>696</v>
+        <v>820</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="2">
-        <v>45686.22916666666</v>
+        <v>45731.22916666666</v>
       </c>
       <c r="B120">
-        <v>696</v>
+        <v>819</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="2">
-        <v>45686.23958333334</v>
+        <v>45731.23958333334</v>
       </c>
       <c r="B121">
-        <v>698</v>
+        <v>823</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="2">
-        <v>45686.25</v>
+        <v>45731.25</v>
       </c>
       <c r="B122">
-        <v>844</v>
+        <v>853</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="2">
-        <v>45686.26041666666</v>
+        <v>45731.26041666666</v>
       </c>
       <c r="B123">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="2">
-        <v>45686.27083333334</v>
+        <v>45731.27083333334</v>
       </c>
       <c r="B124">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="2">
-        <v>45686.28125</v>
+        <v>45731.28125</v>
       </c>
       <c r="B125">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="2">
-        <v>45686.29166666666</v>
+        <v>45731.29166666666</v>
       </c>
       <c r="B126">
-        <v>917</v>
+        <v>850</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="2">
-        <v>45686.30208333334</v>
+        <v>45731.30208333334</v>
       </c>
       <c r="B127">
-        <v>920</v>
+        <v>851</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="2">
-        <v>45686.3125</v>
+        <v>45731.3125</v>
       </c>
       <c r="B128">
-        <v>916</v>
+        <v>850</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="2">
-        <v>45686.32291666666</v>
+        <v>45731.32291666666</v>
       </c>
       <c r="B129">
-        <v>915</v>
+        <v>850</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="2">
-        <v>45686.33333333334</v>
+        <v>45731.33333333334</v>
       </c>
       <c r="B130">
-        <v>933</v>
+        <v>748</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="2">
-        <v>45686.34375</v>
+        <v>45731.34375</v>
       </c>
       <c r="B131">
-        <v>851</v>
+        <v>747</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="2">
-        <v>45686.35416666666</v>
+        <v>45731.35416666666</v>
       </c>
       <c r="B132">
-        <v>850</v>
+        <v>782</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="2">
-        <v>45686.36458333334</v>
+        <v>45731.36458333334</v>
       </c>
       <c r="B133">
-        <v>850</v>
+        <v>781</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="2">
-        <v>45686.375</v>
+        <v>45731.375</v>
       </c>
       <c r="B134">
-        <v>871</v>
+        <v>785</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="2">
-        <v>45686.38541666666</v>
+        <v>45731.38541666666</v>
       </c>
       <c r="B135">
-        <v>863</v>
+        <v>783</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="2">
-        <v>45686.39583333334</v>
+        <v>45731.39583333334</v>
       </c>
       <c r="B136">
-        <v>836</v>
+        <v>782</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="2">
-        <v>45686.40625</v>
+        <v>45731.40625</v>
       </c>
       <c r="B137">
-        <v>835</v>
+        <v>799</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="2">
-        <v>45686.41666666666</v>
+        <v>45731.41666666666</v>
       </c>
       <c r="B138">
-        <v>761</v>
+        <v>775</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="2">
-        <v>45686.42708333334</v>
+        <v>45731.42708333334</v>
       </c>
       <c r="B139">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="2">
-        <v>45686.4375</v>
+        <v>45731.4375</v>
       </c>
       <c r="B140">
-        <v>813</v>
+        <v>761</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="2">
-        <v>45686.44791666666</v>
+        <v>45731.44791666666</v>
       </c>
       <c r="B141">
-        <v>816</v>
+        <v>759</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="2">
-        <v>45686.45833333334</v>
+        <v>45731.45833333334</v>
       </c>
       <c r="B142">
-        <v>813</v>
+        <v>654</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="2">
-        <v>45686.46875</v>
+        <v>45731.46875</v>
       </c>
       <c r="B143">
-        <v>795</v>
+        <v>644</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="2">
-        <v>45686.47916666666</v>
+        <v>45731.47916666666</v>
       </c>
       <c r="B144">
-        <v>795</v>
+        <v>656</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="2">
-        <v>45686.48958333334</v>
+        <v>45731.48958333334</v>
       </c>
       <c r="B145">
-        <v>795</v>
+        <v>656</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="2">
-        <v>45686.5</v>
+        <v>45731.5</v>
       </c>
       <c r="B146">
-        <v>806</v>
+        <v>732</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="2">
-        <v>45686.51041666666</v>
+        <v>45731.51041666666</v>
       </c>
       <c r="B147">
-        <v>805</v>
+        <v>739</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2">
-        <v>45686.52083333334</v>
+        <v>45731.52083333334</v>
       </c>
       <c r="B148">
-        <v>804</v>
+        <v>736</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="2">
-        <v>45686.53125</v>
+        <v>45731.53125</v>
       </c>
       <c r="B149">
-        <v>803</v>
+        <v>737</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="2">
-        <v>45686.54166666666</v>
+        <v>45731.54166666666</v>
       </c>
       <c r="B150">
-        <v>751</v>
+        <v>721</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="2">
-        <v>45686.55208333334</v>
+        <v>45731.55208333334</v>
       </c>
       <c r="B151">
-        <v>751</v>
+        <v>725</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="2">
-        <v>45686.5625</v>
+        <v>45731.5625</v>
       </c>
       <c r="B152">
-        <v>751</v>
+        <v>669</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="2">
-        <v>45686.57291666666</v>
+        <v>45731.57291666666</v>
       </c>
       <c r="B153">
-        <v>754</v>
+        <v>664</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="2">
-        <v>45686.58333333334</v>
+        <v>45731.58333333334</v>
       </c>
       <c r="B154">
-        <v>760</v>
+        <v>669</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="2">
-        <v>45686.59375</v>
+        <v>45731.59375</v>
       </c>
       <c r="B155">
-        <v>759</v>
+        <v>680</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="2">
-        <v>45686.60416666666</v>
+        <v>45731.60416666666</v>
       </c>
       <c r="B156">
-        <v>783</v>
+        <v>681</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="2">
-        <v>45686.61458333334</v>
+        <v>45731.61458333334</v>
       </c>
       <c r="B157">
-        <v>787</v>
+        <v>683</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="2">
-        <v>45686.625</v>
+        <v>45731.625</v>
       </c>
       <c r="B158">
-        <v>824</v>
+        <v>720</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="2">
-        <v>45686.63541666666</v>
+        <v>45731.63541666666</v>
       </c>
       <c r="B159">
-        <v>824</v>
+        <v>726</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="2">
-        <v>45686.64583333334</v>
+        <v>45731.64583333334</v>
       </c>
       <c r="B160">
-        <v>823</v>
+        <v>733</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="2">
-        <v>45686.65625</v>
+        <v>45731.65625</v>
       </c>
       <c r="B161">
-        <v>823</v>
+        <v>727</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="2">
-        <v>45686.66666666666</v>
+        <v>45731.66666666666</v>
       </c>
       <c r="B162">
-        <v>835</v>
+        <v>793</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="2">
-        <v>45686.67708333334</v>
+        <v>45731.67708333334</v>
       </c>
       <c r="B163">
-        <v>837</v>
+        <v>799</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="2">
-        <v>45686.6875</v>
+        <v>45731.6875</v>
       </c>
       <c r="B164">
-        <v>838</v>
+        <v>788</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="2">
-        <v>45686.69791666666</v>
+        <v>45731.69791666666</v>
       </c>
       <c r="B165">
-        <v>842</v>
+        <v>796</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="2">
-        <v>45686.70833333334</v>
+        <v>45731.70833333334</v>
       </c>
       <c r="B166">
-        <v>956</v>
+        <v>883</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="2">
-        <v>45686.71875</v>
+        <v>45731.71875</v>
       </c>
       <c r="B167">
-        <v>966</v>
+        <v>892</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="2">
-        <v>45686.72916666666</v>
+        <v>45731.72916666666</v>
       </c>
       <c r="B168">
-        <v>963</v>
+        <v>902</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="2">
-        <v>45686.73958333334</v>
+        <v>45731.73958333334</v>
       </c>
       <c r="B169">
-        <v>962</v>
+        <v>903</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="2">
-        <v>45686.75</v>
+        <v>45731.75</v>
       </c>
       <c r="B170">
-        <v>977</v>
+        <v>924</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="2">
-        <v>45686.76041666666</v>
+        <v>45731.76041666666</v>
       </c>
       <c r="B171">
-        <v>978</v>
+        <v>932</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="2">
-        <v>45686.77083333334</v>
+        <v>45731.77083333334</v>
       </c>
       <c r="B172">
-        <v>979</v>
+        <v>929</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="2">
-        <v>45686.78125</v>
+        <v>45731.78125</v>
       </c>
       <c r="B173">
-        <v>978</v>
+        <v>935</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="2">
-        <v>45686.79166666666</v>
+        <v>45731.79166666666</v>
       </c>
       <c r="B174">
-        <v>969</v>
+        <v>949</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="2">
-        <v>45686.80208333334</v>
+        <v>45731.80208333334</v>
       </c>
       <c r="B175">
-        <v>966</v>
+        <v>950</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="2">
-        <v>45686.8125</v>
+        <v>45731.8125</v>
       </c>
       <c r="B176">
-        <v>966</v>
+        <v>948</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" s="2">
-        <v>45686.82291666666</v>
+        <v>45731.82291666666</v>
       </c>
       <c r="B177">
-        <v>966</v>
+        <v>947</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="2">
-        <v>45686.83333333334</v>
+        <v>45731.83333333334</v>
       </c>
       <c r="B178">
-        <v>956</v>
+        <v>949</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" s="2">
-        <v>45686.84375</v>
+        <v>45731.84375</v>
       </c>
       <c r="B179">
-        <v>958</v>
+        <v>933</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="2">
-        <v>45686.85416666666</v>
+        <v>45731.85416666666</v>
       </c>
       <c r="B180">
-        <v>959</v>
+        <v>933</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="2">
-        <v>45686.86458333334</v>
+        <v>45731.86458333334</v>
       </c>
       <c r="B181">
-        <v>955</v>
+        <v>932</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="2">
-        <v>45686.875</v>
+        <v>45731.875</v>
       </c>
       <c r="B182">
-        <v>908</v>
+        <v>933</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="2">
-        <v>45686.88541666666</v>
+        <v>45731.88541666666</v>
       </c>
       <c r="B183">
-        <v>906</v>
+        <v>940</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="2">
-        <v>45686.89583333334</v>
+        <v>45731.89583333334</v>
       </c>
       <c r="B184">
-        <v>906</v>
+        <v>942</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="2">
-        <v>45686.90625</v>
+        <v>45731.90625</v>
       </c>
       <c r="B185">
-        <v>905</v>
+        <v>945</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="2">
-        <v>45686.91666666666</v>
+        <v>45731.91666666666</v>
       </c>
       <c r="B186">
-        <v>750</v>
+        <v>868</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="2">
-        <v>45686.92708333334</v>
+        <v>45731.92708333334</v>
       </c>
       <c r="B187">
-        <v>741</v>
+        <v>854</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" s="2">
-        <v>45686.9375</v>
+        <v>45731.9375</v>
       </c>
       <c r="B188">
-        <v>742</v>
+        <v>856</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" s="2">
-        <v>45686.94791666666</v>
+        <v>45731.94791666666</v>
       </c>
       <c r="B189">
-        <v>741</v>
+        <v>857</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="2">
-        <v>45686.95833333334</v>
+        <v>45731.95833333334</v>
       </c>
       <c r="B190">
-        <v>665</v>
+        <v>846</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" s="2">
-        <v>45686.96875</v>
+        <v>45731.96875</v>
       </c>
       <c r="B191">
-        <v>584</v>
+        <v>845</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="2">
-        <v>45686.97916666666</v>
+        <v>45731.97916666666</v>
       </c>
       <c r="B192">
-        <v>584</v>
+        <v>832</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" s="2">
-        <v>45686.98958333334</v>
+        <v>45731.98958333334</v>
       </c>
       <c r="B193">
-        <v>583</v>
+        <v>837</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" s="2">
-        <v>45687</v>
+        <v>45732</v>
       </c>
       <c r="B194">
-        <v>575</v>
+        <v>756</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" s="2">
-        <v>45687.01041666666</v>
+        <v>45732.01041666666</v>
       </c>
       <c r="B195">
-        <v>575</v>
+        <v>750</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" s="2">
-        <v>45687.02083333334</v>
+        <v>45732.02083333334</v>
       </c>
       <c r="B196">
-        <v>576</v>
+        <v>750</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" s="2">
-        <v>45687.03125</v>
+        <v>45732.03125</v>
       </c>
       <c r="B197">
-        <v>576</v>
+        <v>747</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" s="2">
-        <v>45687.04166666666</v>
+        <v>45732.04166666666</v>
       </c>
       <c r="B198">
-        <v>613</v>
+        <v>750</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" s="2">
-        <v>45687.05208333334</v>
+        <v>45732.05208333334</v>
       </c>
       <c r="B199">
-        <v>615</v>
+        <v>749</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" s="2">
-        <v>45687.0625</v>
+        <v>45732.0625</v>
       </c>
       <c r="B200">
-        <v>605</v>
+        <v>748</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" s="2">
-        <v>45687.07291666666</v>
+        <v>45732.07291666666</v>
       </c>
       <c r="B201">
-        <v>604</v>
+        <v>750</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="2">
-        <v>45687.08333333334</v>
+        <v>45732.08333333334</v>
       </c>
       <c r="B202">
-        <v>601</v>
+        <v>750</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" s="2">
-        <v>45687.09375</v>
+        <v>45732.09375</v>
       </c>
       <c r="B203">
-        <v>601</v>
+        <v>749</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" s="2">
-        <v>45687.10416666666</v>
+        <v>45732.10416666666</v>
       </c>
       <c r="B204">
-        <v>602</v>
+        <v>749</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" s="2">
-        <v>45687.11458333334</v>
+        <v>45732.11458333334</v>
       </c>
       <c r="B205">
-        <v>601</v>
+        <v>748</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="2">
-        <v>45687.125</v>
+        <v>45732.125</v>
       </c>
       <c r="B206">
-        <v>601</v>
+        <v>748</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" s="2">
-        <v>45687.13541666666</v>
+        <v>45732.13541666666</v>
       </c>
       <c r="B207">
-        <v>601</v>
+        <v>749</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="2">
-        <v>45687.14583333334</v>
+        <v>45732.14583333334</v>
       </c>
       <c r="B208">
-        <v>601</v>
+        <v>749</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" s="2">
-        <v>45687.15625</v>
+        <v>45732.15625</v>
       </c>
       <c r="B209">
-        <v>601</v>
+        <v>748</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" s="2">
-        <v>45687.16666666666</v>
+        <v>45732.16666666666</v>
       </c>
       <c r="B210">
-        <v>613</v>
+        <v>749</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" s="2">
-        <v>45687.17708333334</v>
+        <v>45732.17708333334</v>
       </c>
       <c r="B211">
-        <v>615</v>
+        <v>750</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" s="2">
-        <v>45687.1875</v>
+        <v>45732.1875</v>
       </c>
       <c r="B212">
-        <v>615</v>
+        <v>750</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" s="2">
-        <v>45687.19791666666</v>
+        <v>45732.19791666666</v>
       </c>
       <c r="B213">
-        <v>620</v>
+        <v>750</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" s="2">
-        <v>45687.20833333334</v>
+        <v>45732.20833333334</v>
       </c>
       <c r="B214">
-        <v>638</v>
+        <v>752</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" s="2">
-        <v>45687.21875</v>
+        <v>45732.21875</v>
       </c>
       <c r="B215">
-        <v>622</v>
+        <v>752</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" s="2">
-        <v>45687.22916666666</v>
+        <v>45732.22916666666</v>
       </c>
       <c r="B216">
-        <v>622</v>
+        <v>752</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" s="2">
-        <v>45687.23958333334</v>
+        <v>45732.23958333334</v>
       </c>
       <c r="B217">
-        <v>625</v>
+        <v>755</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" s="2">
-        <v>45687.25</v>
+        <v>45732.25</v>
       </c>
       <c r="B218">
-        <v>720</v>
+        <v>824</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" s="2">
-        <v>45687.26041666666</v>
+        <v>45732.26041666666</v>
       </c>
       <c r="B219">
-        <v>731</v>
+        <v>830</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" s="2">
-        <v>45687.27083333334</v>
+        <v>45732.27083333334</v>
       </c>
       <c r="B220">
-        <v>786</v>
+        <v>828</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" s="2">
-        <v>45687.28125</v>
+        <v>45732.28125</v>
       </c>
       <c r="B221">
-        <v>784</v>
+        <v>818</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" s="2">
-        <v>45687.29166666666</v>
+        <v>45732.29166666666</v>
       </c>
       <c r="B222">
-        <v>742</v>
+        <v>714</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" s="2">
-        <v>45687.30208333334</v>
+        <v>45732.30208333334</v>
       </c>
       <c r="B223">
-        <v>747</v>
+        <v>711</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" s="2">
-        <v>45687.3125</v>
+        <v>45732.3125</v>
       </c>
       <c r="B224">
-        <v>801</v>
+        <v>712</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" s="2">
-        <v>45687.32291666666</v>
+        <v>45732.32291666666</v>
       </c>
       <c r="B225">
-        <v>802</v>
+        <v>711</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" s="2">
-        <v>45687.33333333334</v>
+        <v>45732.33333333334</v>
       </c>
       <c r="B226">
-        <v>874</v>
+        <v>725</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" s="2">
-        <v>45687.34375</v>
+        <v>45732.34375</v>
       </c>
       <c r="B227">
-        <v>906</v>
+        <v>719</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" s="2">
-        <v>45687.35416666666</v>
+        <v>45732.35416666666</v>
       </c>
       <c r="B228">
-        <v>863</v>
+        <v>720</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" s="2">
-        <v>45687.36458333334</v>
+        <v>45732.36458333334</v>
       </c>
       <c r="B229">
-        <v>860</v>
+        <v>720</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" s="2">
-        <v>45687.375</v>
+        <v>45732.375</v>
       </c>
       <c r="B230">
-        <v>844</v>
+        <v>724</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" s="2">
-        <v>45687.38541666666</v>
+        <v>45732.38541666666</v>
       </c>
       <c r="B231">
-        <v>841</v>
+        <v>720</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" s="2">
-        <v>45687.39583333334</v>
+        <v>45732.39583333334</v>
       </c>
       <c r="B232">
-        <v>840</v>
+        <v>722</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" s="2">
-        <v>45687.40625</v>
+        <v>45732.40625</v>
       </c>
       <c r="B233">
-        <v>891</v>
+        <v>720</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="2">
-        <v>45687.41666666666</v>
+        <v>45732.41666666666</v>
       </c>
       <c r="B234">
-        <v>0</v>
+        <v>646</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235" s="2">
-        <v>45687.42708333334</v>
+        <v>45732.42708333334</v>
       </c>
       <c r="B235">
-        <v>0</v>
+        <v>628</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" s="2">
-        <v>45687.4375</v>
+        <v>45732.4375</v>
       </c>
       <c r="B236">
-        <v>0</v>
+        <v>631</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" s="2">
-        <v>45687.44791666666</v>
+        <v>45732.44791666666</v>
       </c>
       <c r="B237">
-        <v>0</v>
+        <v>628</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" s="2">
-        <v>45687.45833333334</v>
+        <v>45732.45833333334</v>
       </c>
       <c r="B238">
-        <v>0</v>
+        <v>644</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" s="2">
-        <v>45687.46875</v>
+        <v>45732.46875</v>
       </c>
       <c r="B239">
-        <v>0</v>
+        <v>643</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" s="2">
-        <v>45687.47916666666</v>
+        <v>45732.47916666666</v>
       </c>
       <c r="B240">
-        <v>0</v>
+        <v>643</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" s="2">
-        <v>45687.48958333334</v>
+        <v>45732.48958333334</v>
       </c>
       <c r="B241">
-        <v>0</v>
+        <v>646</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" s="2">
-        <v>45687.5</v>
+        <v>45732.5</v>
       </c>
       <c r="B242">
-        <v>0</v>
+        <v>683</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" s="2">
-        <v>45687.51041666666</v>
+        <v>45732.51041666666</v>
       </c>
       <c r="B243">
-        <v>0</v>
+        <v>687</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" s="2">
-        <v>45687.52083333334</v>
+        <v>45732.52083333334</v>
       </c>
       <c r="B244">
-        <v>0</v>
+        <v>689</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" s="2">
-        <v>45687.53125</v>
+        <v>45732.53125</v>
       </c>
       <c r="B245">
-        <v>0</v>
+        <v>686</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" s="2">
-        <v>45687.54166666666</v>
+        <v>45732.54166666666</v>
       </c>
       <c r="B246">
-        <v>0</v>
+        <v>613</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" s="2">
-        <v>45687.55208333334</v>
+        <v>45732.55208333334</v>
       </c>
       <c r="B247">
-        <v>0</v>
+        <v>607</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" s="2">
-        <v>45687.5625</v>
+        <v>45732.5625</v>
       </c>
       <c r="B248">
-        <v>0</v>
+        <v>608</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" s="2">
-        <v>45687.57291666666</v>
+        <v>45732.57291666666</v>
       </c>
       <c r="B249">
-        <v>0</v>
+        <v>608</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" s="2">
-        <v>45687.58333333334</v>
+        <v>45732.58333333334</v>
       </c>
       <c r="B250">
-        <v>0</v>
+        <v>610</v>
       </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251" s="2">
-        <v>45687.59375</v>
+        <v>45732.59375</v>
       </c>
       <c r="B251">
-        <v>0</v>
+        <v>604</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" s="2">
-        <v>45687.60416666666</v>
+        <v>45732.60416666666</v>
       </c>
       <c r="B252">
-        <v>0</v>
+        <v>611</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" s="2">
-        <v>45687.61458333334</v>
+        <v>45732.61458333334</v>
       </c>
       <c r="B253">
-        <v>0</v>
+        <v>612</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" s="2">
-        <v>45687.625</v>
+        <v>45732.625</v>
       </c>
       <c r="B254">
-        <v>0</v>
+        <v>676</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" s="2">
-        <v>45687.63541666666</v>
+        <v>45732.63541666666</v>
       </c>
       <c r="B255">
-        <v>0</v>
+        <v>684</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" s="2">
-        <v>45687.64583333334</v>
+        <v>45732.64583333334</v>
       </c>
       <c r="B256">
-        <v>0</v>
+        <v>686</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257" s="2">
-        <v>45687.65625</v>
+        <v>45732.65625</v>
       </c>
       <c r="B257">
-        <v>0</v>
+        <v>687</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" s="2">
-        <v>45687.66666666666</v>
+        <v>45732.66666666666</v>
       </c>
       <c r="B258">
-        <v>0</v>
+        <v>898</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" s="2">
-        <v>45687.67708333334</v>
+        <v>45732.67708333334</v>
       </c>
       <c r="B259">
-        <v>0</v>
+        <v>916</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" s="2">
-        <v>45687.6875</v>
+        <v>45732.6875</v>
       </c>
       <c r="B260">
-        <v>0</v>
+        <v>921</v>
       </c>
     </row>
     <row r="261" spans="1:2">
       <c r="A261" s="2">
-        <v>45687.69791666666</v>
+        <v>45732.69791666666</v>
       </c>
       <c r="B261">
-        <v>0</v>
+        <v>978</v>
       </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262" s="2">
-        <v>45687.70833333334</v>
+        <v>45732.70833333334</v>
       </c>
       <c r="B262">
-        <v>0</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="263" spans="1:2">
       <c r="A263" s="2">
-        <v>45687.71875</v>
+        <v>45732.71875</v>
       </c>
       <c r="B263">
-        <v>0</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="264" spans="1:2">
       <c r="A264" s="2">
-        <v>45687.72916666666</v>
+        <v>45732.72916666666</v>
       </c>
       <c r="B264">
-        <v>0</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265" s="2">
-        <v>45687.73958333334</v>
+        <v>45732.73958333334</v>
       </c>
       <c r="B265">
-        <v>0</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="266" spans="1:2">
       <c r="A266" s="2">
-        <v>45687.75</v>
+        <v>45732.75</v>
       </c>
       <c r="B266">
-        <v>0</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="A267" s="2">
-        <v>45687.76041666666</v>
+        <v>45732.76041666666</v>
       </c>
       <c r="B267">
-        <v>0</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268" s="2">
-        <v>45687.77083333334</v>
+        <v>45732.77083333334</v>
       </c>
       <c r="B268">
-        <v>0</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="269" spans="1:2">
       <c r="A269" s="2">
-        <v>45687.78125</v>
+        <v>45732.78125</v>
       </c>
       <c r="B269">
-        <v>0</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="270" spans="1:2">
       <c r="A270" s="2">
-        <v>45687.79166666666</v>
+        <v>45732.79166666666</v>
       </c>
       <c r="B270">
-        <v>0</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="271" spans="1:2">
       <c r="A271" s="2">
-        <v>45687.80208333334</v>
+        <v>45732.80208333334</v>
       </c>
       <c r="B271">
-        <v>0</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="272" spans="1:2">
       <c r="A272" s="2">
-        <v>45687.8125</v>
+        <v>45732.8125</v>
       </c>
       <c r="B272">
-        <v>0</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" s="2">
-        <v>45687.82291666666</v>
+        <v>45732.82291666666</v>
       </c>
       <c r="B273">
-        <v>0</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="274" spans="1:2">
       <c r="A274" s="2">
-        <v>45687.83333333334</v>
+        <v>45732.83333333334</v>
       </c>
       <c r="B274">
-        <v>0</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="275" spans="1:2">
       <c r="A275" s="2">
-        <v>45687.84375</v>
+        <v>45732.84375</v>
       </c>
       <c r="B275">
-        <v>0</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="276" spans="1:2">
       <c r="A276" s="2">
-        <v>45687.85416666666</v>
+        <v>45732.85416666666</v>
       </c>
       <c r="B276">
-        <v>0</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="277" spans="1:2">
       <c r="A277" s="2">
-        <v>45687.86458333334</v>
+        <v>45732.86458333334</v>
       </c>
       <c r="B277">
-        <v>0</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="278" spans="1:2">
       <c r="A278" s="2">
-        <v>45687.875</v>
+        <v>45732.875</v>
       </c>
       <c r="B278">
-        <v>0</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="279" spans="1:2">
       <c r="A279" s="2">
-        <v>45687.88541666666</v>
+        <v>45732.88541666666</v>
       </c>
       <c r="B279">
-        <v>0</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="280" spans="1:2">
       <c r="A280" s="2">
-        <v>45687.89583333334</v>
+        <v>45732.89583333334</v>
       </c>
       <c r="B280">
-        <v>0</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="281" spans="1:2">
       <c r="A281" s="2">
-        <v>45687.90625</v>
+        <v>45732.90625</v>
       </c>
       <c r="B281">
-        <v>0</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="282" spans="1:2">
       <c r="A282" s="2">
-        <v>45687.91666666666</v>
+        <v>45732.91666666666</v>
       </c>
       <c r="B282">
-        <v>0</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="283" spans="1:2">
       <c r="A283" s="2">
-        <v>45687.92708333334</v>
+        <v>45732.92708333334</v>
       </c>
       <c r="B283">
-        <v>0</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="284" spans="1:2">
       <c r="A284" s="2">
-        <v>45687.9375</v>
+        <v>45732.9375</v>
       </c>
       <c r="B284">
-        <v>0</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="285" spans="1:2">
       <c r="A285" s="2">
-        <v>45687.94791666666</v>
+        <v>45732.94791666666</v>
       </c>
       <c r="B285">
-        <v>0</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="286" spans="1:2">
       <c r="A286" s="2">
-        <v>45687.95833333334</v>
+        <v>45732.95833333334</v>
       </c>
       <c r="B286">
-        <v>0</v>
+        <v>937</v>
       </c>
     </row>
     <row r="287" spans="1:2">
       <c r="A287" s="2">
-        <v>45687.96875</v>
+        <v>45732.96875</v>
       </c>
       <c r="B287">
-        <v>0</v>
+        <v>932</v>
       </c>
     </row>
     <row r="288" spans="1:2">
       <c r="A288" s="2">
-        <v>45687.97916666666</v>
+        <v>45732.97916666666</v>
       </c>
       <c r="B288">
-        <v>0</v>
+        <v>932</v>
       </c>
     </row>
     <row r="289" spans="1:2">
       <c r="A289" s="2">
-        <v>45687.98958333334</v>
+        <v>45732.98958333334</v>
       </c>
       <c r="B289">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2">
+      <c r="A290" s="2">
+        <v>45733</v>
+      </c>
+      <c r="B290">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2">
+      <c r="A291" s="2">
+        <v>45733.01041666666</v>
+      </c>
+      <c r="B291">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2">
+      <c r="A292" s="2">
+        <v>45733.02083333334</v>
+      </c>
+      <c r="B292">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2">
+      <c r="A293" s="2">
+        <v>45733.03125</v>
+      </c>
+      <c r="B293">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2">
+      <c r="A294" s="2">
+        <v>45733.04166666666</v>
+      </c>
+      <c r="B294">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2">
+      <c r="A295" s="2">
+        <v>45733.05208333334</v>
+      </c>
+      <c r="B295">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2">
+      <c r="A296" s="2">
+        <v>45733.0625</v>
+      </c>
+      <c r="B296">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2">
+      <c r="A297" s="2">
+        <v>45733.07291666666</v>
+      </c>
+      <c r="B297">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2">
+      <c r="A298" s="2">
+        <v>45733.08333333334</v>
+      </c>
+      <c r="B298">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2">
+      <c r="A299" s="2">
+        <v>45733.09375</v>
+      </c>
+      <c r="B299">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2">
+      <c r="A300" s="2">
+        <v>45733.10416666666</v>
+      </c>
+      <c r="B300">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2">
+      <c r="A301" s="2">
+        <v>45733.11458333334</v>
+      </c>
+      <c r="B301">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2">
+      <c r="A302" s="2">
+        <v>45733.125</v>
+      </c>
+      <c r="B302">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2">
+      <c r="A303" s="2">
+        <v>45733.13541666666</v>
+      </c>
+      <c r="B303">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2">
+      <c r="A304" s="2">
+        <v>45733.14583333334</v>
+      </c>
+      <c r="B304">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2">
+      <c r="A305" s="2">
+        <v>45733.15625</v>
+      </c>
+      <c r="B305">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2">
+      <c r="A306" s="2">
+        <v>45733.16666666666</v>
+      </c>
+      <c r="B306">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2">
+      <c r="A307" s="2">
+        <v>45733.17708333334</v>
+      </c>
+      <c r="B307">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2">
+      <c r="A308" s="2">
+        <v>45733.1875</v>
+      </c>
+      <c r="B308">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2">
+      <c r="A309" s="2">
+        <v>45733.19791666666</v>
+      </c>
+      <c r="B309">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2">
+      <c r="A310" s="2">
+        <v>45733.20833333334</v>
+      </c>
+      <c r="B310">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2">
+      <c r="A311" s="2">
+        <v>45733.21875</v>
+      </c>
+      <c r="B311">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2">
+      <c r="A312" s="2">
+        <v>45733.22916666666</v>
+      </c>
+      <c r="B312">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2">
+      <c r="A313" s="2">
+        <v>45733.23958333334</v>
+      </c>
+      <c r="B313">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2">
+      <c r="A314" s="2">
+        <v>45733.25</v>
+      </c>
+      <c r="B314">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2">
+      <c r="A315" s="2">
+        <v>45733.26041666666</v>
+      </c>
+      <c r="B315">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2">
+      <c r="A316" s="2">
+        <v>45733.27083333334</v>
+      </c>
+      <c r="B316">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2">
+      <c r="A317" s="2">
+        <v>45733.28125</v>
+      </c>
+      <c r="B317">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2">
+      <c r="A318" s="2">
+        <v>45733.29166666666</v>
+      </c>
+      <c r="B318">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2">
+      <c r="A319" s="2">
+        <v>45733.30208333334</v>
+      </c>
+      <c r="B319">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2">
+      <c r="A320" s="2">
+        <v>45733.3125</v>
+      </c>
+      <c r="B320">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2">
+      <c r="A321" s="2">
+        <v>45733.32291666666</v>
+      </c>
+      <c r="B321">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2">
+      <c r="A322" s="2">
+        <v>45733.33333333334</v>
+      </c>
+      <c r="B322">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2">
+      <c r="A323" s="2">
+        <v>45733.34375</v>
+      </c>
+      <c r="B323">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2">
+      <c r="A324" s="2">
+        <v>45733.35416666666</v>
+      </c>
+      <c r="B324">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2">
+      <c r="A325" s="2">
+        <v>45733.36458333334</v>
+      </c>
+      <c r="B325">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2">
+      <c r="A326" s="2">
+        <v>45733.375</v>
+      </c>
+      <c r="B326">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2">
+      <c r="A327" s="2">
+        <v>45733.38541666666</v>
+      </c>
+      <c r="B327">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2">
+      <c r="A328" s="2">
+        <v>45733.39583333334</v>
+      </c>
+      <c r="B328">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2">
+      <c r="A329" s="2">
+        <v>45733.40625</v>
+      </c>
+      <c r="B329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2">
+      <c r="A330" s="2">
+        <v>45733.41666666666</v>
+      </c>
+      <c r="B330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2">
+      <c r="A331" s="2">
+        <v>45733.42708333334</v>
+      </c>
+      <c r="B331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2">
+      <c r="A332" s="2">
+        <v>45733.4375</v>
+      </c>
+      <c r="B332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2">
+      <c r="A333" s="2">
+        <v>45733.44791666666</v>
+      </c>
+      <c r="B333">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2">
+      <c r="A334" s="2">
+        <v>45733.45833333334</v>
+      </c>
+      <c r="B334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2">
+      <c r="A335" s="2">
+        <v>45733.46875</v>
+      </c>
+      <c r="B335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2">
+      <c r="A336" s="2">
+        <v>45733.47916666666</v>
+      </c>
+      <c r="B336">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2">
+      <c r="A337" s="2">
+        <v>45733.48958333334</v>
+      </c>
+      <c r="B337">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2">
+      <c r="A338" s="2">
+        <v>45733.5</v>
+      </c>
+      <c r="B338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2">
+      <c r="A339" s="2">
+        <v>45733.51041666666</v>
+      </c>
+      <c r="B339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2">
+      <c r="A340" s="2">
+        <v>45733.52083333334</v>
+      </c>
+      <c r="B340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2">
+      <c r="A341" s="2">
+        <v>45733.53125</v>
+      </c>
+      <c r="B341">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2">
+      <c r="A342" s="2">
+        <v>45733.54166666666</v>
+      </c>
+      <c r="B342">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2">
+      <c r="A343" s="2">
+        <v>45733.55208333334</v>
+      </c>
+      <c r="B343">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2">
+      <c r="A344" s="2">
+        <v>45733.5625</v>
+      </c>
+      <c r="B344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2">
+      <c r="A345" s="2">
+        <v>45733.57291666666</v>
+      </c>
+      <c r="B345">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2">
+      <c r="A346" s="2">
+        <v>45733.58333333334</v>
+      </c>
+      <c r="B346">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2">
+      <c r="A347" s="2">
+        <v>45733.59375</v>
+      </c>
+      <c r="B347">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2">
+      <c r="A348" s="2">
+        <v>45733.60416666666</v>
+      </c>
+      <c r="B348">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2">
+      <c r="A349" s="2">
+        <v>45733.61458333334</v>
+      </c>
+      <c r="B349">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2">
+      <c r="A350" s="2">
+        <v>45733.625</v>
+      </c>
+      <c r="B350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2">
+      <c r="A351" s="2">
+        <v>45733.63541666666</v>
+      </c>
+      <c r="B351">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2">
+      <c r="A352" s="2">
+        <v>45733.64583333334</v>
+      </c>
+      <c r="B352">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2">
+      <c r="A353" s="2">
+        <v>45733.65625</v>
+      </c>
+      <c r="B353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2">
+      <c r="A354" s="2">
+        <v>45733.66666666666</v>
+      </c>
+      <c r="B354">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2">
+      <c r="A355" s="2">
+        <v>45733.67708333334</v>
+      </c>
+      <c r="B355">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2">
+      <c r="A356" s="2">
+        <v>45733.6875</v>
+      </c>
+      <c r="B356">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2">
+      <c r="A357" s="2">
+        <v>45733.69791666666</v>
+      </c>
+      <c r="B357">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2">
+      <c r="A358" s="2">
+        <v>45733.70833333334</v>
+      </c>
+      <c r="B358">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2">
+      <c r="A359" s="2">
+        <v>45733.71875</v>
+      </c>
+      <c r="B359">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2">
+      <c r="A360" s="2">
+        <v>45733.72916666666</v>
+      </c>
+      <c r="B360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2">
+      <c r="A361" s="2">
+        <v>45733.73958333334</v>
+      </c>
+      <c r="B361">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2">
+      <c r="A362" s="2">
+        <v>45733.75</v>
+      </c>
+      <c r="B362">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2">
+      <c r="A363" s="2">
+        <v>45733.76041666666</v>
+      </c>
+      <c r="B363">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2">
+      <c r="A364" s="2">
+        <v>45733.77083333334</v>
+      </c>
+      <c r="B364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2">
+      <c r="A365" s="2">
+        <v>45733.78125</v>
+      </c>
+      <c r="B365">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2">
+      <c r="A366" s="2">
+        <v>45733.79166666666</v>
+      </c>
+      <c r="B366">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2">
+      <c r="A367" s="2">
+        <v>45733.80208333334</v>
+      </c>
+      <c r="B367">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2">
+      <c r="A368" s="2">
+        <v>45733.8125</v>
+      </c>
+      <c r="B368">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2">
+      <c r="A369" s="2">
+        <v>45733.82291666666</v>
+      </c>
+      <c r="B369">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2">
+      <c r="A370" s="2">
+        <v>45733.83333333334</v>
+      </c>
+      <c r="B370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2">
+      <c r="A371" s="2">
+        <v>45733.84375</v>
+      </c>
+      <c r="B371">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2">
+      <c r="A372" s="2">
+        <v>45733.85416666666</v>
+      </c>
+      <c r="B372">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2">
+      <c r="A373" s="2">
+        <v>45733.86458333334</v>
+      </c>
+      <c r="B373">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2">
+      <c r="A374" s="2">
+        <v>45733.875</v>
+      </c>
+      <c r="B374">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2">
+      <c r="A375" s="2">
+        <v>45733.88541666666</v>
+      </c>
+      <c r="B375">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2">
+      <c r="A376" s="2">
+        <v>45733.89583333334</v>
+      </c>
+      <c r="B376">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2">
+      <c r="A377" s="2">
+        <v>45733.90625</v>
+      </c>
+      <c r="B377">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2">
+      <c r="A378" s="2">
+        <v>45733.91666666666</v>
+      </c>
+      <c r="B378">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2">
+      <c r="A379" s="2">
+        <v>45733.92708333334</v>
+      </c>
+      <c r="B379">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2">
+      <c r="A380" s="2">
+        <v>45733.9375</v>
+      </c>
+      <c r="B380">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2">
+      <c r="A381" s="2">
+        <v>45733.94791666666</v>
+      </c>
+      <c r="B381">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2">
+      <c r="A382" s="2">
+        <v>45733.95833333334</v>
+      </c>
+      <c r="B382">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2">
+      <c r="A383" s="2">
+        <v>45733.96875</v>
+      </c>
+      <c r="B383">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2">
+      <c r="A384" s="2">
+        <v>45733.97916666666</v>
+      </c>
+      <c r="B384">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2">
+      <c r="A385" s="2">
+        <v>45733.98958333334</v>
+      </c>
+      <c r="B385">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding a fallback to the entsoe fetching functions
</commit_message>
<xml_diff>
--- a/data_fetching/Entsoe/Actual_Production_Hydro_River.xlsx
+++ b/data_fetching/Entsoe/Actual_Production_Hydro_River.xlsx
@@ -381,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B385"/>
+  <dimension ref="A1:B481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3016,7 +3016,7 @@
         <v>45733.40625</v>
       </c>
       <c r="B329">
-        <v>0</v>
+        <v>964</v>
       </c>
     </row>
     <row r="330" spans="1:2">
@@ -3024,7 +3024,7 @@
         <v>45733.41666666666</v>
       </c>
       <c r="B330">
-        <v>0</v>
+        <v>946</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -3032,7 +3032,7 @@
         <v>45733.42708333334</v>
       </c>
       <c r="B331">
-        <v>0</v>
+        <v>947</v>
       </c>
     </row>
     <row r="332" spans="1:2">
@@ -3040,7 +3040,7 @@
         <v>45733.4375</v>
       </c>
       <c r="B332">
-        <v>0</v>
+        <v>947</v>
       </c>
     </row>
     <row r="333" spans="1:2">
@@ -3048,7 +3048,7 @@
         <v>45733.44791666666</v>
       </c>
       <c r="B333">
-        <v>0</v>
+        <v>945</v>
       </c>
     </row>
     <row r="334" spans="1:2">
@@ -3056,7 +3056,7 @@
         <v>45733.45833333334</v>
       </c>
       <c r="B334">
-        <v>0</v>
+        <v>942</v>
       </c>
     </row>
     <row r="335" spans="1:2">
@@ -3064,7 +3064,7 @@
         <v>45733.46875</v>
       </c>
       <c r="B335">
-        <v>0</v>
+        <v>968</v>
       </c>
     </row>
     <row r="336" spans="1:2">
@@ -3072,7 +3072,7 @@
         <v>45733.47916666666</v>
       </c>
       <c r="B336">
-        <v>0</v>
+        <v>985</v>
       </c>
     </row>
     <row r="337" spans="1:2">
@@ -3080,7 +3080,7 @@
         <v>45733.48958333334</v>
       </c>
       <c r="B337">
-        <v>0</v>
+        <v>981</v>
       </c>
     </row>
     <row r="338" spans="1:2">
@@ -3088,7 +3088,7 @@
         <v>45733.5</v>
       </c>
       <c r="B338">
-        <v>0</v>
+        <v>882</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -3096,7 +3096,7 @@
         <v>45733.51041666666</v>
       </c>
       <c r="B339">
-        <v>0</v>
+        <v>903</v>
       </c>
     </row>
     <row r="340" spans="1:2">
@@ -3104,7 +3104,7 @@
         <v>45733.52083333334</v>
       </c>
       <c r="B340">
-        <v>0</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="341" spans="1:2">
@@ -3112,7 +3112,7 @@
         <v>45733.53125</v>
       </c>
       <c r="B341">
-        <v>0</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="342" spans="1:2">
@@ -3120,7 +3120,7 @@
         <v>45733.54166666666</v>
       </c>
       <c r="B342">
-        <v>0</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="343" spans="1:2">
@@ -3128,7 +3128,7 @@
         <v>45733.55208333334</v>
       </c>
       <c r="B343">
-        <v>0</v>
+        <v>995</v>
       </c>
     </row>
     <row r="344" spans="1:2">
@@ -3136,7 +3136,7 @@
         <v>45733.5625</v>
       </c>
       <c r="B344">
-        <v>0</v>
+        <v>965</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -3144,7 +3144,7 @@
         <v>45733.57291666666</v>
       </c>
       <c r="B345">
-        <v>0</v>
+        <v>958</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -3152,7 +3152,7 @@
         <v>45733.58333333334</v>
       </c>
       <c r="B346">
-        <v>0</v>
+        <v>855</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -3160,7 +3160,7 @@
         <v>45733.59375</v>
       </c>
       <c r="B347">
-        <v>0</v>
+        <v>850</v>
       </c>
     </row>
     <row r="348" spans="1:2">
@@ -3168,7 +3168,7 @@
         <v>45733.60416666666</v>
       </c>
       <c r="B348">
-        <v>0</v>
+        <v>849</v>
       </c>
     </row>
     <row r="349" spans="1:2">
@@ -3176,7 +3176,7 @@
         <v>45733.61458333334</v>
       </c>
       <c r="B349">
-        <v>0</v>
+        <v>858</v>
       </c>
     </row>
     <row r="350" spans="1:2">
@@ -3184,7 +3184,7 @@
         <v>45733.625</v>
       </c>
       <c r="B350">
-        <v>0</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="351" spans="1:2">
@@ -3192,7 +3192,7 @@
         <v>45733.63541666666</v>
       </c>
       <c r="B351">
-        <v>0</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="352" spans="1:2">
@@ -3200,7 +3200,7 @@
         <v>45733.64583333334</v>
       </c>
       <c r="B352">
-        <v>0</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -3208,7 +3208,7 @@
         <v>45733.65625</v>
       </c>
       <c r="B353">
-        <v>0</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="354" spans="1:2">
@@ -3216,7 +3216,7 @@
         <v>45733.66666666666</v>
       </c>
       <c r="B354">
-        <v>0</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -3224,7 +3224,7 @@
         <v>45733.67708333334</v>
       </c>
       <c r="B355">
-        <v>0</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="356" spans="1:2">
@@ -3232,7 +3232,7 @@
         <v>45733.6875</v>
       </c>
       <c r="B356">
-        <v>0</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="357" spans="1:2">
@@ -3240,7 +3240,7 @@
         <v>45733.69791666666</v>
       </c>
       <c r="B357">
-        <v>0</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="358" spans="1:2">
@@ -3248,7 +3248,7 @@
         <v>45733.70833333334</v>
       </c>
       <c r="B358">
-        <v>0</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="359" spans="1:2">
@@ -3256,7 +3256,7 @@
         <v>45733.71875</v>
       </c>
       <c r="B359">
-        <v>0</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -3264,7 +3264,7 @@
         <v>45733.72916666666</v>
       </c>
       <c r="B360">
-        <v>0</v>
+        <v>928</v>
       </c>
     </row>
     <row r="361" spans="1:2">
@@ -3272,7 +3272,7 @@
         <v>45733.73958333334</v>
       </c>
       <c r="B361">
-        <v>0</v>
+        <v>901</v>
       </c>
     </row>
     <row r="362" spans="1:2">
@@ -3280,7 +3280,7 @@
         <v>45733.75</v>
       </c>
       <c r="B362">
-        <v>0</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="363" spans="1:2">
@@ -3288,7 +3288,7 @@
         <v>45733.76041666666</v>
       </c>
       <c r="B363">
-        <v>0</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="364" spans="1:2">
@@ -3296,7 +3296,7 @@
         <v>45733.77083333334</v>
       </c>
       <c r="B364">
-        <v>0</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="365" spans="1:2">
@@ -3304,7 +3304,7 @@
         <v>45733.78125</v>
       </c>
       <c r="B365">
-        <v>0</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="366" spans="1:2">
@@ -3312,7 +3312,7 @@
         <v>45733.79166666666</v>
       </c>
       <c r="B366">
-        <v>0</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="367" spans="1:2">
@@ -3320,7 +3320,7 @@
         <v>45733.80208333334</v>
       </c>
       <c r="B367">
-        <v>0</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="368" spans="1:2">
@@ -3328,7 +3328,7 @@
         <v>45733.8125</v>
       </c>
       <c r="B368">
-        <v>0</v>
+        <v>999</v>
       </c>
     </row>
     <row r="369" spans="1:2">
@@ -3336,7 +3336,7 @@
         <v>45733.82291666666</v>
       </c>
       <c r="B369">
-        <v>0</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="370" spans="1:2">
@@ -3344,7 +3344,7 @@
         <v>45733.83333333334</v>
       </c>
       <c r="B370">
-        <v>0</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="371" spans="1:2">
@@ -3352,7 +3352,7 @@
         <v>45733.84375</v>
       </c>
       <c r="B371">
-        <v>0</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="372" spans="1:2">
@@ -3360,7 +3360,7 @@
         <v>45733.85416666666</v>
       </c>
       <c r="B372">
-        <v>0</v>
+        <v>941</v>
       </c>
     </row>
     <row r="373" spans="1:2">
@@ -3368,7 +3368,7 @@
         <v>45733.86458333334</v>
       </c>
       <c r="B373">
-        <v>0</v>
+        <v>939</v>
       </c>
     </row>
     <row r="374" spans="1:2">
@@ -3376,7 +3376,7 @@
         <v>45733.875</v>
       </c>
       <c r="B374">
-        <v>0</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="375" spans="1:2">
@@ -3384,7 +3384,7 @@
         <v>45733.88541666666</v>
       </c>
       <c r="B375">
-        <v>0</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="376" spans="1:2">
@@ -3392,7 +3392,7 @@
         <v>45733.89583333334</v>
       </c>
       <c r="B376">
-        <v>0</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="377" spans="1:2">
@@ -3400,7 +3400,7 @@
         <v>45733.90625</v>
       </c>
       <c r="B377">
-        <v>0</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="378" spans="1:2">
@@ -3408,7 +3408,7 @@
         <v>45733.91666666666</v>
       </c>
       <c r="B378">
-        <v>0</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="379" spans="1:2">
@@ -3416,7 +3416,7 @@
         <v>45733.92708333334</v>
       </c>
       <c r="B379">
-        <v>0</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="380" spans="1:2">
@@ -3424,7 +3424,7 @@
         <v>45733.9375</v>
       </c>
       <c r="B380">
-        <v>0</v>
+        <v>964</v>
       </c>
     </row>
     <row r="381" spans="1:2">
@@ -3432,7 +3432,7 @@
         <v>45733.94791666666</v>
       </c>
       <c r="B381">
-        <v>0</v>
+        <v>960</v>
       </c>
     </row>
     <row r="382" spans="1:2">
@@ -3440,7 +3440,7 @@
         <v>45733.95833333334</v>
       </c>
       <c r="B382">
-        <v>0</v>
+        <v>981</v>
       </c>
     </row>
     <row r="383" spans="1:2">
@@ -3448,7 +3448,7 @@
         <v>45733.96875</v>
       </c>
       <c r="B383">
-        <v>0</v>
+        <v>993</v>
       </c>
     </row>
     <row r="384" spans="1:2">
@@ -3456,7 +3456,7 @@
         <v>45733.97916666666</v>
       </c>
       <c r="B384">
-        <v>0</v>
+        <v>994</v>
       </c>
     </row>
     <row r="385" spans="1:2">
@@ -3464,6 +3464,774 @@
         <v>45733.98958333334</v>
       </c>
       <c r="B385">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2">
+      <c r="A386" s="2">
+        <v>45734</v>
+      </c>
+      <c r="B386">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2">
+      <c r="A387" s="2">
+        <v>45734.01041666666</v>
+      </c>
+      <c r="B387">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2">
+      <c r="A388" s="2">
+        <v>45734.02083333334</v>
+      </c>
+      <c r="B388">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2">
+      <c r="A389" s="2">
+        <v>45734.03125</v>
+      </c>
+      <c r="B389">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2">
+      <c r="A390" s="2">
+        <v>45734.04166666666</v>
+      </c>
+      <c r="B390">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2">
+      <c r="A391" s="2">
+        <v>45734.05208333334</v>
+      </c>
+      <c r="B391">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2">
+      <c r="A392" s="2">
+        <v>45734.0625</v>
+      </c>
+      <c r="B392">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2">
+      <c r="A393" s="2">
+        <v>45734.07291666666</v>
+      </c>
+      <c r="B393">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2">
+      <c r="A394" s="2">
+        <v>45734.08333333334</v>
+      </c>
+      <c r="B394">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2">
+      <c r="A395" s="2">
+        <v>45734.09375</v>
+      </c>
+      <c r="B395">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2">
+      <c r="A396" s="2">
+        <v>45734.10416666666</v>
+      </c>
+      <c r="B396">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2">
+      <c r="A397" s="2">
+        <v>45734.11458333334</v>
+      </c>
+      <c r="B397">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2">
+      <c r="A398" s="2">
+        <v>45734.125</v>
+      </c>
+      <c r="B398">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2">
+      <c r="A399" s="2">
+        <v>45734.13541666666</v>
+      </c>
+      <c r="B399">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2">
+      <c r="A400" s="2">
+        <v>45734.14583333334</v>
+      </c>
+      <c r="B400">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2">
+      <c r="A401" s="2">
+        <v>45734.15625</v>
+      </c>
+      <c r="B401">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2">
+      <c r="A402" s="2">
+        <v>45734.16666666666</v>
+      </c>
+      <c r="B402">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2">
+      <c r="A403" s="2">
+        <v>45734.17708333334</v>
+      </c>
+      <c r="B403">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2">
+      <c r="A404" s="2">
+        <v>45734.1875</v>
+      </c>
+      <c r="B404">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2">
+      <c r="A405" s="2">
+        <v>45734.19791666666</v>
+      </c>
+      <c r="B405">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2">
+      <c r="A406" s="2">
+        <v>45734.20833333334</v>
+      </c>
+      <c r="B406">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2">
+      <c r="A407" s="2">
+        <v>45734.21875</v>
+      </c>
+      <c r="B407">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2">
+      <c r="A408" s="2">
+        <v>45734.22916666666</v>
+      </c>
+      <c r="B408">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2">
+      <c r="A409" s="2">
+        <v>45734.23958333334</v>
+      </c>
+      <c r="B409">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2">
+      <c r="A410" s="2">
+        <v>45734.25</v>
+      </c>
+      <c r="B410">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2">
+      <c r="A411" s="2">
+        <v>45734.26041666666</v>
+      </c>
+      <c r="B411">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2">
+      <c r="A412" s="2">
+        <v>45734.27083333334</v>
+      </c>
+      <c r="B412">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2">
+      <c r="A413" s="2">
+        <v>45734.28125</v>
+      </c>
+      <c r="B413">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2">
+      <c r="A414" s="2">
+        <v>45734.29166666666</v>
+      </c>
+      <c r="B414">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2">
+      <c r="A415" s="2">
+        <v>45734.30208333334</v>
+      </c>
+      <c r="B415">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2">
+      <c r="A416" s="2">
+        <v>45734.3125</v>
+      </c>
+      <c r="B416">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2">
+      <c r="A417" s="2">
+        <v>45734.32291666666</v>
+      </c>
+      <c r="B417">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2">
+      <c r="A418" s="2">
+        <v>45734.33333333334</v>
+      </c>
+      <c r="B418">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2">
+      <c r="A419" s="2">
+        <v>45734.34375</v>
+      </c>
+      <c r="B419">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2">
+      <c r="A420" s="2">
+        <v>45734.35416666666</v>
+      </c>
+      <c r="B420">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2">
+      <c r="A421" s="2">
+        <v>45734.36458333334</v>
+      </c>
+      <c r="B421">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2">
+      <c r="A422" s="2">
+        <v>45734.375</v>
+      </c>
+      <c r="B422">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2">
+      <c r="A423" s="2">
+        <v>45734.38541666666</v>
+      </c>
+      <c r="B423">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2">
+      <c r="A424" s="2">
+        <v>45734.39583333334</v>
+      </c>
+      <c r="B424">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2">
+      <c r="A425" s="2">
+        <v>45734.40625</v>
+      </c>
+      <c r="B425">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2">
+      <c r="A426" s="2">
+        <v>45734.41666666666</v>
+      </c>
+      <c r="B426">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2">
+      <c r="A427" s="2">
+        <v>45734.42708333334</v>
+      </c>
+      <c r="B427">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2">
+      <c r="A428" s="2">
+        <v>45734.4375</v>
+      </c>
+      <c r="B428">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2">
+      <c r="A429" s="2">
+        <v>45734.44791666666</v>
+      </c>
+      <c r="B429">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2">
+      <c r="A430" s="2">
+        <v>45734.45833333334</v>
+      </c>
+      <c r="B430">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2">
+      <c r="A431" s="2">
+        <v>45734.46875</v>
+      </c>
+      <c r="B431">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2">
+      <c r="A432" s="2">
+        <v>45734.47916666666</v>
+      </c>
+      <c r="B432">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2">
+      <c r="A433" s="2">
+        <v>45734.48958333334</v>
+      </c>
+      <c r="B433">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2">
+      <c r="A434" s="2">
+        <v>45734.5</v>
+      </c>
+      <c r="B434">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2">
+      <c r="A435" s="2">
+        <v>45734.51041666666</v>
+      </c>
+      <c r="B435">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2">
+      <c r="A436" s="2">
+        <v>45734.52083333334</v>
+      </c>
+      <c r="B436">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2">
+      <c r="A437" s="2">
+        <v>45734.53125</v>
+      </c>
+      <c r="B437">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2">
+      <c r="A438" s="2">
+        <v>45734.54166666666</v>
+      </c>
+      <c r="B438">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2">
+      <c r="A439" s="2">
+        <v>45734.55208333334</v>
+      </c>
+      <c r="B439">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2">
+      <c r="A440" s="2">
+        <v>45734.5625</v>
+      </c>
+      <c r="B440">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2">
+      <c r="A441" s="2">
+        <v>45734.57291666666</v>
+      </c>
+      <c r="B441">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2">
+      <c r="A442" s="2">
+        <v>45734.58333333334</v>
+      </c>
+      <c r="B442">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2">
+      <c r="A443" s="2">
+        <v>45734.59375</v>
+      </c>
+      <c r="B443">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2">
+      <c r="A444" s="2">
+        <v>45734.60416666666</v>
+      </c>
+      <c r="B444">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2">
+      <c r="A445" s="2">
+        <v>45734.61458333334</v>
+      </c>
+      <c r="B445">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2">
+      <c r="A446" s="2">
+        <v>45734.625</v>
+      </c>
+      <c r="B446">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2">
+      <c r="A447" s="2">
+        <v>45734.63541666666</v>
+      </c>
+      <c r="B447">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2">
+      <c r="A448" s="2">
+        <v>45734.64583333334</v>
+      </c>
+      <c r="B448">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2">
+      <c r="A449" s="2">
+        <v>45734.65625</v>
+      </c>
+      <c r="B449">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2">
+      <c r="A450" s="2">
+        <v>45734.66666666666</v>
+      </c>
+      <c r="B450">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2">
+      <c r="A451" s="2">
+        <v>45734.67708333334</v>
+      </c>
+      <c r="B451">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2">
+      <c r="A452" s="2">
+        <v>45734.6875</v>
+      </c>
+      <c r="B452">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2">
+      <c r="A453" s="2">
+        <v>45734.69791666666</v>
+      </c>
+      <c r="B453">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2">
+      <c r="A454" s="2">
+        <v>45734.70833333334</v>
+      </c>
+      <c r="B454">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2">
+      <c r="A455" s="2">
+        <v>45734.71875</v>
+      </c>
+      <c r="B455">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2">
+      <c r="A456" s="2">
+        <v>45734.72916666666</v>
+      </c>
+      <c r="B456">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2">
+      <c r="A457" s="2">
+        <v>45734.73958333334</v>
+      </c>
+      <c r="B457">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2">
+      <c r="A458" s="2">
+        <v>45734.75</v>
+      </c>
+      <c r="B458">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2">
+      <c r="A459" s="2">
+        <v>45734.76041666666</v>
+      </c>
+      <c r="B459">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2">
+      <c r="A460" s="2">
+        <v>45734.77083333334</v>
+      </c>
+      <c r="B460">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2">
+      <c r="A461" s="2">
+        <v>45734.78125</v>
+      </c>
+      <c r="B461">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2">
+      <c r="A462" s="2">
+        <v>45734.79166666666</v>
+      </c>
+      <c r="B462">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2">
+      <c r="A463" s="2">
+        <v>45734.80208333334</v>
+      </c>
+      <c r="B463">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2">
+      <c r="A464" s="2">
+        <v>45734.8125</v>
+      </c>
+      <c r="B464">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2">
+      <c r="A465" s="2">
+        <v>45734.82291666666</v>
+      </c>
+      <c r="B465">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2">
+      <c r="A466" s="2">
+        <v>45734.83333333334</v>
+      </c>
+      <c r="B466">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2">
+      <c r="A467" s="2">
+        <v>45734.84375</v>
+      </c>
+      <c r="B467">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2">
+      <c r="A468" s="2">
+        <v>45734.85416666666</v>
+      </c>
+      <c r="B468">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2">
+      <c r="A469" s="2">
+        <v>45734.86458333334</v>
+      </c>
+      <c r="B469">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2">
+      <c r="A470" s="2">
+        <v>45734.875</v>
+      </c>
+      <c r="B470">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2">
+      <c r="A471" s="2">
+        <v>45734.88541666666</v>
+      </c>
+      <c r="B471">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2">
+      <c r="A472" s="2">
+        <v>45734.89583333334</v>
+      </c>
+      <c r="B472">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2">
+      <c r="A473" s="2">
+        <v>45734.90625</v>
+      </c>
+      <c r="B473">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2">
+      <c r="A474" s="2">
+        <v>45734.91666666666</v>
+      </c>
+      <c r="B474">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2">
+      <c r="A475" s="2">
+        <v>45734.92708333334</v>
+      </c>
+      <c r="B475">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2">
+      <c r="A476" s="2">
+        <v>45734.9375</v>
+      </c>
+      <c r="B476">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2">
+      <c r="A477" s="2">
+        <v>45734.94791666666</v>
+      </c>
+      <c r="B477">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2">
+      <c r="A478" s="2">
+        <v>45734.95833333334</v>
+      </c>
+      <c r="B478">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2">
+      <c r="A479" s="2">
+        <v>45734.96875</v>
+      </c>
+      <c r="B479">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2">
+      <c r="A480" s="2">
+        <v>45734.97916666666</v>
+      </c>
+      <c r="B480">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2">
+      <c r="A481" s="2">
+        <v>45734.98958333334</v>
+      </c>
+      <c r="B481">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changing Astro location to Dabaca
</commit_message>
<xml_diff>
--- a/data_fetching/Entsoe/Actual_Production_Hydro_River.xlsx
+++ b/data_fetching/Entsoe/Actual_Production_Hydro_River.xlsx
@@ -381,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B289"/>
+  <dimension ref="A1:B193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -397,2305 +397,1537 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>45797</v>
+        <v>45806</v>
       </c>
       <c r="B2">
-        <v>946</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>45797.01041666666</v>
+        <v>45806.01041666666</v>
       </c>
       <c r="B3">
-        <v>910</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>45797.02083333334</v>
+        <v>45806.02083333334</v>
       </c>
       <c r="B4">
-        <v>909</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>45797.03125</v>
+        <v>45806.03125</v>
       </c>
       <c r="B5">
-        <v>909</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>45797.04166666666</v>
+        <v>45806.04166666666</v>
       </c>
       <c r="B6">
-        <v>922</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>45797.05208333334</v>
+        <v>45806.05208333334</v>
       </c>
       <c r="B7">
-        <v>921</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>45797.0625</v>
+        <v>45806.0625</v>
       </c>
       <c r="B8">
-        <v>919</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>45797.07291666666</v>
+        <v>45806.07291666666</v>
       </c>
       <c r="B9">
-        <v>896</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>45797.08333333334</v>
+        <v>45806.08333333334</v>
       </c>
       <c r="B10">
-        <v>887</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>45797.09375</v>
+        <v>45806.09375</v>
       </c>
       <c r="B11">
-        <v>885</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>45797.10416666666</v>
+        <v>45806.10416666666</v>
       </c>
       <c r="B12">
-        <v>885</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>45797.11458333334</v>
+        <v>45806.11458333334</v>
       </c>
       <c r="B13">
-        <v>909</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>45797.125</v>
+        <v>45806.125</v>
       </c>
       <c r="B14">
-        <v>874</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>45797.13541666666</v>
+        <v>45806.13541666666</v>
       </c>
       <c r="B15">
-        <v>864</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>45797.14583333334</v>
+        <v>45806.14583333334</v>
       </c>
       <c r="B16">
-        <v>864</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>45797.15625</v>
+        <v>45806.15625</v>
       </c>
       <c r="B17">
-        <v>865</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>45797.16666666666</v>
+        <v>45806.16666666666</v>
       </c>
       <c r="B18">
-        <v>887</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>45797.17708333334</v>
+        <v>45806.17708333334</v>
       </c>
       <c r="B19">
-        <v>891</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>45797.1875</v>
+        <v>45806.1875</v>
       </c>
       <c r="B20">
-        <v>911</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>45797.19791666666</v>
+        <v>45806.19791666666</v>
       </c>
       <c r="B21">
-        <v>918</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>45797.20833333334</v>
+        <v>45806.20833333334</v>
       </c>
       <c r="B22">
-        <v>919</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>45797.21875</v>
+        <v>45806.21875</v>
       </c>
       <c r="B23">
-        <v>924</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>45797.22916666666</v>
+        <v>45806.22916666666</v>
       </c>
       <c r="B24">
-        <v>936</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>45797.23958333334</v>
+        <v>45806.23958333334</v>
       </c>
       <c r="B25">
-        <v>943</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>45797.25</v>
+        <v>45806.25</v>
       </c>
       <c r="B26">
-        <v>1095</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
-        <v>45797.26041666666</v>
+        <v>45806.26041666666</v>
       </c>
       <c r="B27">
-        <v>1158</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
-        <v>45797.27083333334</v>
+        <v>45806.27083333334</v>
       </c>
       <c r="B28">
-        <v>1157</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
-        <v>45797.28125</v>
+        <v>45806.28125</v>
       </c>
       <c r="B29">
-        <v>1155</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2">
-        <v>45797.29166666666</v>
+        <v>45806.29166666666</v>
       </c>
       <c r="B30">
-        <v>1113</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2">
-        <v>45797.30208333334</v>
+        <v>45806.30208333334</v>
       </c>
       <c r="B31">
-        <v>1082</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2">
-        <v>45797.3125</v>
+        <v>45806.3125</v>
       </c>
       <c r="B32">
-        <v>1090</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2">
-        <v>45797.32291666666</v>
+        <v>45806.32291666666</v>
       </c>
       <c r="B33">
-        <v>1092</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2">
-        <v>45797.33333333334</v>
+        <v>45806.33333333334</v>
       </c>
       <c r="B34">
-        <v>1084</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2">
-        <v>45797.34375</v>
+        <v>45806.34375</v>
       </c>
       <c r="B35">
-        <v>1077</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2">
-        <v>45797.35416666666</v>
+        <v>45806.35416666666</v>
       </c>
       <c r="B36">
-        <v>1058</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2">
-        <v>45797.36458333334</v>
+        <v>45806.36458333334</v>
       </c>
       <c r="B37">
-        <v>989</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2">
-        <v>45797.375</v>
+        <v>45806.375</v>
       </c>
       <c r="B38">
-        <v>642</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2">
-        <v>45797.38541666666</v>
+        <v>45806.38541666666</v>
       </c>
       <c r="B39">
-        <v>576</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2">
-        <v>45797.39583333334</v>
+        <v>45806.39583333334</v>
       </c>
       <c r="B40">
-        <v>568</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2">
-        <v>45797.40625</v>
+        <v>45806.40625</v>
       </c>
       <c r="B41">
-        <v>568</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2">
-        <v>45797.41666666666</v>
+        <v>45806.41666666666</v>
       </c>
       <c r="B42">
-        <v>733</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2">
-        <v>45797.42708333334</v>
+        <v>45806.42708333334</v>
       </c>
       <c r="B43">
-        <v>737</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2">
-        <v>45797.4375</v>
+        <v>45806.4375</v>
       </c>
       <c r="B44">
-        <v>736</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2">
-        <v>45797.44791666666</v>
+        <v>45806.44791666666</v>
       </c>
       <c r="B45">
-        <v>734</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2">
-        <v>45797.45833333334</v>
+        <v>45806.45833333334</v>
       </c>
       <c r="B46">
-        <v>710</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2">
-        <v>45797.46875</v>
+        <v>45806.46875</v>
       </c>
       <c r="B47">
-        <v>707</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2">
-        <v>45797.47916666666</v>
+        <v>45806.47916666666</v>
       </c>
       <c r="B48">
-        <v>664</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2">
-        <v>45797.48958333334</v>
+        <v>45806.48958333334</v>
       </c>
       <c r="B49">
-        <v>659</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2">
-        <v>45797.5</v>
+        <v>45806.5</v>
       </c>
       <c r="B50">
-        <v>866</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2">
-        <v>45797.51041666666</v>
+        <v>45806.51041666666</v>
       </c>
       <c r="B51">
-        <v>830</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2">
-        <v>45797.52083333334</v>
+        <v>45806.52083333334</v>
       </c>
       <c r="B52">
-        <v>826</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2">
-        <v>45797.53125</v>
+        <v>45806.53125</v>
       </c>
       <c r="B53">
-        <v>941</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2">
-        <v>45797.54166666666</v>
+        <v>45806.54166666666</v>
       </c>
       <c r="B54">
-        <v>908</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2">
-        <v>45797.55208333334</v>
+        <v>45806.55208333334</v>
       </c>
       <c r="B55">
-        <v>909</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2">
-        <v>45797.5625</v>
+        <v>45806.5625</v>
       </c>
       <c r="B56">
-        <v>910</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2">
-        <v>45797.57291666666</v>
+        <v>45806.57291666666</v>
       </c>
       <c r="B57">
-        <v>912</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2">
-        <v>45797.58333333334</v>
+        <v>45806.58333333334</v>
       </c>
       <c r="B58">
-        <v>1044</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2">
-        <v>45797.59375</v>
+        <v>45806.59375</v>
       </c>
       <c r="B59">
-        <v>1032</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2">
-        <v>45797.60416666666</v>
+        <v>45806.60416666666</v>
       </c>
       <c r="B60">
-        <v>1017</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2">
-        <v>45797.61458333334</v>
+        <v>45806.61458333334</v>
       </c>
       <c r="B61">
-        <v>1015</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2">
-        <v>45797.625</v>
+        <v>45806.625</v>
       </c>
       <c r="B62">
-        <v>1028</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2">
-        <v>45797.63541666666</v>
+        <v>45806.63541666666</v>
       </c>
       <c r="B63">
-        <v>1036</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2">
-        <v>45797.64583333334</v>
+        <v>45806.64583333334</v>
       </c>
       <c r="B64">
-        <v>1157</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2">
-        <v>45797.65625</v>
+        <v>45806.65625</v>
       </c>
       <c r="B65">
-        <v>1181</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2">
-        <v>45797.66666666666</v>
+        <v>45806.66666666666</v>
       </c>
       <c r="B66">
-        <v>1180</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2">
-        <v>45797.67708333334</v>
+        <v>45806.67708333334</v>
       </c>
       <c r="B67">
-        <v>1123</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2">
-        <v>45797.6875</v>
+        <v>45806.6875</v>
       </c>
       <c r="B68">
-        <v>1159</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2">
-        <v>45797.69791666666</v>
+        <v>45806.69791666666</v>
       </c>
       <c r="B69">
-        <v>1172</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2">
-        <v>45797.70833333334</v>
+        <v>45806.70833333334</v>
       </c>
       <c r="B70">
-        <v>1199</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2">
-        <v>45797.71875</v>
+        <v>45806.71875</v>
       </c>
       <c r="B71">
-        <v>1251</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="2">
-        <v>45797.72916666666</v>
+        <v>45806.72916666666</v>
       </c>
       <c r="B72">
-        <v>1255</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2">
-        <v>45797.73958333334</v>
+        <v>45806.73958333334</v>
       </c>
       <c r="B73">
-        <v>1267</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="2">
-        <v>45797.75</v>
+        <v>45806.75</v>
       </c>
       <c r="B74">
-        <v>1270</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="2">
-        <v>45797.76041666666</v>
+        <v>45806.76041666666</v>
       </c>
       <c r="B75">
-        <v>1275</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="2">
-        <v>45797.77083333334</v>
+        <v>45806.77083333334</v>
       </c>
       <c r="B76">
-        <v>1282</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="2">
-        <v>45797.78125</v>
+        <v>45806.78125</v>
       </c>
       <c r="B77">
-        <v>1306</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="2">
-        <v>45797.79166666666</v>
+        <v>45806.79166666666</v>
       </c>
       <c r="B78">
-        <v>1222</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="2">
-        <v>45797.80208333334</v>
+        <v>45806.80208333334</v>
       </c>
       <c r="B79">
-        <v>1213</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="2">
-        <v>45797.8125</v>
+        <v>45806.8125</v>
       </c>
       <c r="B80">
-        <v>1205</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="2">
-        <v>45797.82291666666</v>
+        <v>45806.82291666666</v>
       </c>
       <c r="B81">
-        <v>1205</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="2">
-        <v>45797.83333333334</v>
+        <v>45806.83333333334</v>
       </c>
       <c r="B82">
-        <v>1263</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="2">
-        <v>45797.84375</v>
+        <v>45806.84375</v>
       </c>
       <c r="B83">
-        <v>1269</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="2">
-        <v>45797.85416666666</v>
+        <v>45806.85416666666</v>
       </c>
       <c r="B84">
-        <v>1270</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="2">
-        <v>45797.86458333334</v>
+        <v>45806.86458333334</v>
       </c>
       <c r="B85">
-        <v>1269</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="2">
-        <v>45797.875</v>
+        <v>45806.875</v>
       </c>
       <c r="B86">
-        <v>1264</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="2">
-        <v>45797.88541666666</v>
+        <v>45806.88541666666</v>
       </c>
       <c r="B87">
-        <v>1258</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="2">
-        <v>45797.89583333334</v>
+        <v>45806.89583333334</v>
       </c>
       <c r="B88">
-        <v>1258</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="2">
-        <v>45797.90625</v>
+        <v>45806.90625</v>
       </c>
       <c r="B89">
-        <v>1254</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="2">
-        <v>45797.91666666666</v>
+        <v>45806.91666666666</v>
       </c>
       <c r="B90">
-        <v>1188</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="2">
-        <v>45797.92708333334</v>
+        <v>45806.92708333334</v>
       </c>
       <c r="B91">
-        <v>1176</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="2">
-        <v>45797.9375</v>
+        <v>45806.9375</v>
       </c>
       <c r="B92">
-        <v>1179</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="2">
-        <v>45797.94791666666</v>
+        <v>45806.94791666666</v>
       </c>
       <c r="B93">
-        <v>1177</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="2">
-        <v>45797.95833333334</v>
+        <v>45806.95833333334</v>
       </c>
       <c r="B94">
-        <v>1173</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="2">
-        <v>45797.96875</v>
+        <v>45806.96875</v>
       </c>
       <c r="B95">
-        <v>1165</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="2">
-        <v>45797.97916666666</v>
+        <v>45806.97916666666</v>
       </c>
       <c r="B96">
-        <v>1162</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="2">
-        <v>45797.98958333334</v>
+        <v>45806.98958333334</v>
       </c>
       <c r="B97">
-        <v>1160</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="2">
-        <v>45798</v>
+        <v>45807</v>
       </c>
       <c r="B98">
-        <v>1080</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="2">
-        <v>45798.01041666666</v>
+        <v>45807.01041666666</v>
       </c>
       <c r="B99">
-        <v>1035</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="2">
-        <v>45798.02083333334</v>
+        <v>45807.02083333334</v>
       </c>
       <c r="B100">
-        <v>1034</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="2">
-        <v>45798.03125</v>
+        <v>45807.03125</v>
       </c>
       <c r="B101">
-        <v>1034</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="2">
-        <v>45798.04166666666</v>
+        <v>45807.04166666666</v>
       </c>
       <c r="B102">
-        <v>1031</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="2">
-        <v>45798.05208333334</v>
+        <v>45807.05208333334</v>
       </c>
       <c r="B103">
-        <v>1032</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="2">
-        <v>45798.0625</v>
+        <v>45807.0625</v>
       </c>
       <c r="B104">
-        <v>1030</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="2">
-        <v>45798.07291666666</v>
+        <v>45807.07291666666</v>
       </c>
       <c r="B105">
-        <v>1026</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="2">
-        <v>45798.08333333334</v>
+        <v>45807.08333333334</v>
       </c>
       <c r="B106">
-        <v>1031</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="2">
-        <v>45798.09375</v>
+        <v>45807.09375</v>
       </c>
       <c r="B107">
-        <v>1031</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="2">
-        <v>45798.10416666666</v>
+        <v>45807.10416666666</v>
       </c>
       <c r="B108">
-        <v>1031</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="2">
-        <v>45798.11458333334</v>
+        <v>45807.11458333334</v>
       </c>
       <c r="B109">
-        <v>1031</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="2">
-        <v>45798.125</v>
+        <v>45807.125</v>
       </c>
       <c r="B110">
-        <v>1049</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="2">
-        <v>45798.13541666666</v>
+        <v>45807.13541666666</v>
       </c>
       <c r="B111">
-        <v>1046</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="2">
-        <v>45798.14583333334</v>
+        <v>45807.14583333334</v>
       </c>
       <c r="B112">
-        <v>1044</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="2">
-        <v>45798.15625</v>
+        <v>45807.15625</v>
       </c>
       <c r="B113">
-        <v>1042</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="2">
-        <v>45798.16666666666</v>
+        <v>45807.16666666666</v>
       </c>
       <c r="B114">
-        <v>1041</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="2">
-        <v>45798.17708333334</v>
+        <v>45807.17708333334</v>
       </c>
       <c r="B115">
-        <v>1044</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="2">
-        <v>45798.1875</v>
+        <v>45807.1875</v>
       </c>
       <c r="B116">
-        <v>1045</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="2">
-        <v>45798.19791666666</v>
+        <v>45807.19791666666</v>
       </c>
       <c r="B117">
-        <v>1046</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="2">
-        <v>45798.20833333334</v>
+        <v>45807.20833333334</v>
       </c>
       <c r="B118">
-        <v>1034</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="2">
-        <v>45798.21875</v>
+        <v>45807.21875</v>
       </c>
       <c r="B119">
-        <v>1009</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="2">
-        <v>45798.22916666666</v>
+        <v>45807.22916666666</v>
       </c>
       <c r="B120">
-        <v>999</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="2">
-        <v>45798.23958333334</v>
+        <v>45807.23958333334</v>
       </c>
       <c r="B121">
-        <v>999</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="2">
-        <v>45798.25</v>
+        <v>45807.25</v>
       </c>
       <c r="B122">
-        <v>1028</v>
+        <v>1866</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="2">
-        <v>45798.26041666666</v>
+        <v>45807.26041666666</v>
       </c>
       <c r="B123">
-        <v>1031</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="2">
-        <v>45798.27083333334</v>
+        <v>45807.27083333334</v>
       </c>
       <c r="B124">
-        <v>1030</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="2">
-        <v>45798.28125</v>
+        <v>45807.28125</v>
       </c>
       <c r="B125">
-        <v>1029</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="2">
-        <v>45798.29166666666</v>
+        <v>45807.29166666666</v>
       </c>
       <c r="B126">
-        <v>1036</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="2">
-        <v>45798.30208333334</v>
+        <v>45807.30208333334</v>
       </c>
       <c r="B127">
-        <v>1032</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="2">
-        <v>45798.3125</v>
+        <v>45807.3125</v>
       </c>
       <c r="B128">
-        <v>1033</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="2">
-        <v>45798.32291666666</v>
+        <v>45807.32291666666</v>
       </c>
       <c r="B129">
-        <v>1030</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="2">
-        <v>45798.33333333334</v>
+        <v>45807.33333333334</v>
       </c>
       <c r="B130">
-        <v>1069</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="2">
-        <v>45798.34375</v>
+        <v>45807.34375</v>
       </c>
       <c r="B131">
-        <v>1070</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="2">
-        <v>45798.35416666666</v>
+        <v>45807.35416666666</v>
       </c>
       <c r="B132">
-        <v>1069</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="2">
-        <v>45798.36458333334</v>
+        <v>45807.36458333334</v>
       </c>
       <c r="B133">
-        <v>1060</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="2">
-        <v>45798.375</v>
+        <v>45807.375</v>
       </c>
       <c r="B134">
-        <v>1034</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="2">
-        <v>45798.38541666666</v>
+        <v>45807.38541666666</v>
       </c>
       <c r="B135">
-        <v>1029</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="2">
-        <v>45798.39583333334</v>
+        <v>45807.39583333334</v>
       </c>
       <c r="B136">
-        <v>1027</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="2">
-        <v>45798.40625</v>
+        <v>45807.40625</v>
       </c>
       <c r="B137">
-        <v>1030</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="2">
-        <v>45798.41666666666</v>
+        <v>45807.41666666666</v>
       </c>
       <c r="B138">
-        <v>1047</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="2">
-        <v>45798.42708333334</v>
+        <v>45807.42708333334</v>
       </c>
       <c r="B139">
-        <v>1049</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="2">
-        <v>45798.4375</v>
+        <v>45807.4375</v>
       </c>
       <c r="B140">
-        <v>1050</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="2">
-        <v>45798.44791666666</v>
+        <v>45807.44791666666</v>
       </c>
       <c r="B141">
-        <v>1004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="2">
-        <v>45798.45833333334</v>
+        <v>45807.45833333334</v>
       </c>
       <c r="B142">
-        <v>1009</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="2">
-        <v>45798.46875</v>
+        <v>45807.46875</v>
       </c>
       <c r="B143">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="2">
-        <v>45798.47916666666</v>
+        <v>45807.47916666666</v>
       </c>
       <c r="B144">
-        <v>1001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="2">
-        <v>45798.48958333334</v>
+        <v>45807.48958333334</v>
       </c>
       <c r="B145">
-        <v>1001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="2">
-        <v>45798.5</v>
+        <v>45807.5</v>
       </c>
       <c r="B146">
-        <v>988</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="2">
-        <v>45798.51041666666</v>
+        <v>45807.51041666666</v>
       </c>
       <c r="B147">
-        <v>962</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2">
-        <v>45798.52083333334</v>
+        <v>45807.52083333334</v>
       </c>
       <c r="B148">
-        <v>1007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="2">
-        <v>45798.53125</v>
+        <v>45807.53125</v>
       </c>
       <c r="B149">
-        <v>1065</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="2">
-        <v>45798.54166666666</v>
+        <v>45807.54166666666</v>
       </c>
       <c r="B150">
-        <v>1042</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="2">
-        <v>45798.55208333334</v>
+        <v>45807.55208333334</v>
       </c>
       <c r="B151">
-        <v>999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="2">
-        <v>45798.5625</v>
+        <v>45807.5625</v>
       </c>
       <c r="B152">
-        <v>998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="2">
-        <v>45798.57291666666</v>
+        <v>45807.57291666666</v>
       </c>
       <c r="B153">
-        <v>999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="2">
-        <v>45798.58333333334</v>
+        <v>45807.58333333334</v>
       </c>
       <c r="B154">
-        <v>982</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="2">
-        <v>45798.59375</v>
+        <v>45807.59375</v>
       </c>
       <c r="B155">
-        <v>982</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="2">
-        <v>45798.60416666666</v>
+        <v>45807.60416666666</v>
       </c>
       <c r="B156">
-        <v>1077</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="2">
-        <v>45798.61458333334</v>
+        <v>45807.61458333334</v>
       </c>
       <c r="B157">
-        <v>1109</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="2">
-        <v>45798.625</v>
+        <v>45807.625</v>
       </c>
       <c r="B158">
-        <v>1177</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="2">
-        <v>45798.63541666666</v>
+        <v>45807.63541666666</v>
       </c>
       <c r="B159">
-        <v>1191</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="2">
-        <v>45798.64583333334</v>
+        <v>45807.64583333334</v>
       </c>
       <c r="B160">
-        <v>1188</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="2">
-        <v>45798.65625</v>
+        <v>45807.65625</v>
       </c>
       <c r="B161">
-        <v>1194</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="2">
-        <v>45798.66666666666</v>
+        <v>45807.66666666666</v>
       </c>
       <c r="B162">
-        <v>1101</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="2">
-        <v>45798.67708333334</v>
+        <v>45807.67708333334</v>
       </c>
       <c r="B163">
-        <v>1115</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="2">
-        <v>45798.6875</v>
+        <v>45807.6875</v>
       </c>
       <c r="B164">
-        <v>1135</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="2">
-        <v>45798.69791666666</v>
+        <v>45807.69791666666</v>
       </c>
       <c r="B165">
-        <v>1137</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="2">
-        <v>45798.70833333334</v>
+        <v>45807.70833333334</v>
       </c>
       <c r="B166">
-        <v>1195</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="2">
-        <v>45798.71875</v>
+        <v>45807.71875</v>
       </c>
       <c r="B167">
-        <v>1202</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="2">
-        <v>45798.72916666666</v>
+        <v>45807.72916666666</v>
       </c>
       <c r="B168">
-        <v>1209</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="2">
-        <v>45798.73958333334</v>
+        <v>45807.73958333334</v>
       </c>
       <c r="B169">
-        <v>1209</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="2">
-        <v>45798.75</v>
+        <v>45807.75</v>
       </c>
       <c r="B170">
-        <v>1305</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="2">
-        <v>45798.76041666666</v>
+        <v>45807.76041666666</v>
       </c>
       <c r="B171">
-        <v>1338</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="2">
-        <v>45798.77083333334</v>
+        <v>45807.77083333334</v>
       </c>
       <c r="B172">
-        <v>1330</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="2">
-        <v>45798.78125</v>
+        <v>45807.78125</v>
       </c>
       <c r="B173">
-        <v>1328</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="2">
-        <v>45798.79166666666</v>
+        <v>45807.79166666666</v>
       </c>
       <c r="B174">
-        <v>1349</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="2">
-        <v>45798.80208333334</v>
+        <v>45807.80208333334</v>
       </c>
       <c r="B175">
-        <v>1350</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="2">
-        <v>45798.8125</v>
+        <v>45807.8125</v>
       </c>
       <c r="B176">
-        <v>1350</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" s="2">
-        <v>45798.82291666666</v>
+        <v>45807.82291666666</v>
       </c>
       <c r="B177">
-        <v>1349</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="2">
-        <v>45798.83333333334</v>
+        <v>45807.83333333334</v>
       </c>
       <c r="B178">
-        <v>1386</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" s="2">
-        <v>45798.84375</v>
+        <v>45807.84375</v>
       </c>
       <c r="B179">
-        <v>1393</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="2">
-        <v>45798.85416666666</v>
+        <v>45807.85416666666</v>
       </c>
       <c r="B180">
-        <v>1390</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="2">
-        <v>45798.86458333334</v>
+        <v>45807.86458333334</v>
       </c>
       <c r="B181">
-        <v>1378</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="2">
-        <v>45798.875</v>
+        <v>45807.875</v>
       </c>
       <c r="B182">
-        <v>1346</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="2">
-        <v>45798.88541666666</v>
+        <v>45807.88541666666</v>
       </c>
       <c r="B183">
-        <v>1346</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="2">
-        <v>45798.89583333334</v>
+        <v>45807.89583333334</v>
       </c>
       <c r="B184">
-        <v>1346</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="2">
-        <v>45798.90625</v>
+        <v>45807.90625</v>
       </c>
       <c r="B185">
-        <v>1343</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="2">
-        <v>45798.91666666666</v>
+        <v>45807.91666666666</v>
       </c>
       <c r="B186">
-        <v>1291</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="2">
-        <v>45798.92708333334</v>
+        <v>45807.92708333334</v>
       </c>
       <c r="B187">
-        <v>1278</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" s="2">
-        <v>45798.9375</v>
+        <v>45807.9375</v>
       </c>
       <c r="B188">
-        <v>1282</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" s="2">
-        <v>45798.94791666666</v>
+        <v>45807.94791666666</v>
       </c>
       <c r="B189">
-        <v>1269</v>
+        <v>0</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="2">
-        <v>45798.95833333334</v>
+        <v>45807.95833333334</v>
       </c>
       <c r="B190">
-        <v>1088</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" s="2">
-        <v>45798.96875</v>
+        <v>45807.96875</v>
       </c>
       <c r="B191">
-        <v>1083</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="2">
-        <v>45798.97916666666</v>
+        <v>45807.97916666666</v>
       </c>
       <c r="B192">
-        <v>1084</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" s="2">
-        <v>45798.98958333334</v>
+        <v>45807.98958333334</v>
       </c>
       <c r="B193">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2">
-      <c r="A194" s="2">
-        <v>45799</v>
-      </c>
-      <c r="B194">
-        <v>1058</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2">
-      <c r="A195" s="2">
-        <v>45799.01041666666</v>
-      </c>
-      <c r="B195">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2">
-      <c r="A196" s="2">
-        <v>45799.02083333334</v>
-      </c>
-      <c r="B196">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2">
-      <c r="A197" s="2">
-        <v>45799.03125</v>
-      </c>
-      <c r="B197">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2">
-      <c r="A198" s="2">
-        <v>45799.04166666666</v>
-      </c>
-      <c r="B198">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2">
-      <c r="A199" s="2">
-        <v>45799.05208333334</v>
-      </c>
-      <c r="B199">
-        <v>1068</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2">
-      <c r="A200" s="2">
-        <v>45799.0625</v>
-      </c>
-      <c r="B200">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2">
-      <c r="A201" s="2">
-        <v>45799.07291666666</v>
-      </c>
-      <c r="B201">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2">
-      <c r="A202" s="2">
-        <v>45799.08333333334</v>
-      </c>
-      <c r="B202">
-        <v>1078</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2">
-      <c r="A203" s="2">
-        <v>45799.09375</v>
-      </c>
-      <c r="B203">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2">
-      <c r="A204" s="2">
-        <v>45799.10416666666</v>
-      </c>
-      <c r="B204">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2">
-      <c r="A205" s="2">
-        <v>45799.11458333334</v>
-      </c>
-      <c r="B205">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2">
-      <c r="A206" s="2">
-        <v>45799.125</v>
-      </c>
-      <c r="B206">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2">
-      <c r="A207" s="2">
-        <v>45799.13541666666</v>
-      </c>
-      <c r="B207">
-        <v>1058</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2">
-      <c r="A208" s="2">
-        <v>45799.14583333334</v>
-      </c>
-      <c r="B208">
-        <v>1057</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2">
-      <c r="A209" s="2">
-        <v>45799.15625</v>
-      </c>
-      <c r="B209">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2">
-      <c r="A210" s="2">
-        <v>45799.16666666666</v>
-      </c>
-      <c r="B210">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2">
-      <c r="A211" s="2">
-        <v>45799.17708333334</v>
-      </c>
-      <c r="B211">
-        <v>1114</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2">
-      <c r="A212" s="2">
-        <v>45799.1875</v>
-      </c>
-      <c r="B212">
-        <v>1121</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2">
-      <c r="A213" s="2">
-        <v>45799.19791666666</v>
-      </c>
-      <c r="B213">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2">
-      <c r="A214" s="2">
-        <v>45799.20833333334</v>
-      </c>
-      <c r="B214">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2">
-      <c r="A215" s="2">
-        <v>45799.21875</v>
-      </c>
-      <c r="B215">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2">
-      <c r="A216" s="2">
-        <v>45799.22916666666</v>
-      </c>
-      <c r="B216">
-        <v>1155</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2">
-      <c r="A217" s="2">
-        <v>45799.23958333334</v>
-      </c>
-      <c r="B217">
-        <v>1165</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2">
-      <c r="A218" s="2">
-        <v>45799.25</v>
-      </c>
-      <c r="B218">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2">
-      <c r="A219" s="2">
-        <v>45799.26041666666</v>
-      </c>
-      <c r="B219">
-        <v>1335</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2">
-      <c r="A220" s="2">
-        <v>45799.27083333334</v>
-      </c>
-      <c r="B220">
-        <v>1338</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2">
-      <c r="A221" s="2">
-        <v>45799.28125</v>
-      </c>
-      <c r="B221">
-        <v>1335</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2">
-      <c r="A222" s="2">
-        <v>45799.29166666666</v>
-      </c>
-      <c r="B222">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2">
-      <c r="A223" s="2">
-        <v>45799.30208333334</v>
-      </c>
-      <c r="B223">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2">
-      <c r="A224" s="2">
-        <v>45799.3125</v>
-      </c>
-      <c r="B224">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2">
-      <c r="A225" s="2">
-        <v>45799.32291666666</v>
-      </c>
-      <c r="B225">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2">
-      <c r="A226" s="2">
-        <v>45799.33333333334</v>
-      </c>
-      <c r="B226">
-        <v>1365</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2">
-      <c r="A227" s="2">
-        <v>45799.34375</v>
-      </c>
-      <c r="B227">
-        <v>1368</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2">
-      <c r="A228" s="2">
-        <v>45799.35416666666</v>
-      </c>
-      <c r="B228">
-        <v>1363</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2">
-      <c r="A229" s="2">
-        <v>45799.36458333334</v>
-      </c>
-      <c r="B229">
-        <v>1363</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2">
-      <c r="A230" s="2">
-        <v>45799.375</v>
-      </c>
-      <c r="B230">
-        <v>1325</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2">
-      <c r="A231" s="2">
-        <v>45799.38541666666</v>
-      </c>
-      <c r="B231">
-        <v>1184</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2">
-      <c r="A232" s="2">
-        <v>45799.39583333334</v>
-      </c>
-      <c r="B232">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2">
-      <c r="A233" s="2">
-        <v>45799.40625</v>
-      </c>
-      <c r="B233">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2">
-      <c r="A234" s="2">
-        <v>45799.41666666666</v>
-      </c>
-      <c r="B234">
-        <v>1133</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2">
-      <c r="A235" s="2">
-        <v>45799.42708333334</v>
-      </c>
-      <c r="B235">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2">
-      <c r="A236" s="2">
-        <v>45799.4375</v>
-      </c>
-      <c r="B236">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2">
-      <c r="A237" s="2">
-        <v>45799.44791666666</v>
-      </c>
-      <c r="B237">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2">
-      <c r="A238" s="2">
-        <v>45799.45833333334</v>
-      </c>
-      <c r="B238">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2">
-      <c r="A239" s="2">
-        <v>45799.46875</v>
-      </c>
-      <c r="B239">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2">
-      <c r="A240" s="2">
-        <v>45799.47916666666</v>
-      </c>
-      <c r="B240">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2">
-      <c r="A241" s="2">
-        <v>45799.48958333334</v>
-      </c>
-      <c r="B241">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2">
-      <c r="A242" s="2">
-        <v>45799.5</v>
-      </c>
-      <c r="B242">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2">
-      <c r="A243" s="2">
-        <v>45799.51041666666</v>
-      </c>
-      <c r="B243">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2">
-      <c r="A244" s="2">
-        <v>45799.52083333334</v>
-      </c>
-      <c r="B244">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2">
-      <c r="A245" s="2">
-        <v>45799.53125</v>
-      </c>
-      <c r="B245">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2">
-      <c r="A246" s="2">
-        <v>45799.54166666666</v>
-      </c>
-      <c r="B246">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2">
-      <c r="A247" s="2">
-        <v>45799.55208333334</v>
-      </c>
-      <c r="B247">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2">
-      <c r="A248" s="2">
-        <v>45799.5625</v>
-      </c>
-      <c r="B248">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2">
-      <c r="A249" s="2">
-        <v>45799.57291666666</v>
-      </c>
-      <c r="B249">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2">
-      <c r="A250" s="2">
-        <v>45799.58333333334</v>
-      </c>
-      <c r="B250">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2">
-      <c r="A251" s="2">
-        <v>45799.59375</v>
-      </c>
-      <c r="B251">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2">
-      <c r="A252" s="2">
-        <v>45799.60416666666</v>
-      </c>
-      <c r="B252">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2">
-      <c r="A253" s="2">
-        <v>45799.61458333334</v>
-      </c>
-      <c r="B253">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2">
-      <c r="A254" s="2">
-        <v>45799.625</v>
-      </c>
-      <c r="B254">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2">
-      <c r="A255" s="2">
-        <v>45799.63541666666</v>
-      </c>
-      <c r="B255">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2">
-      <c r="A256" s="2">
-        <v>45799.64583333334</v>
-      </c>
-      <c r="B256">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2">
-      <c r="A257" s="2">
-        <v>45799.65625</v>
-      </c>
-      <c r="B257">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2">
-      <c r="A258" s="2">
-        <v>45799.66666666666</v>
-      </c>
-      <c r="B258">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2">
-      <c r="A259" s="2">
-        <v>45799.67708333334</v>
-      </c>
-      <c r="B259">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2">
-      <c r="A260" s="2">
-        <v>45799.6875</v>
-      </c>
-      <c r="B260">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2">
-      <c r="A261" s="2">
-        <v>45799.69791666666</v>
-      </c>
-      <c r="B261">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2">
-      <c r="A262" s="2">
-        <v>45799.70833333334</v>
-      </c>
-      <c r="B262">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2">
-      <c r="A263" s="2">
-        <v>45799.71875</v>
-      </c>
-      <c r="B263">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2">
-      <c r="A264" s="2">
-        <v>45799.72916666666</v>
-      </c>
-      <c r="B264">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2">
-      <c r="A265" s="2">
-        <v>45799.73958333334</v>
-      </c>
-      <c r="B265">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2">
-      <c r="A266" s="2">
-        <v>45799.75</v>
-      </c>
-      <c r="B266">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2">
-      <c r="A267" s="2">
-        <v>45799.76041666666</v>
-      </c>
-      <c r="B267">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2">
-      <c r="A268" s="2">
-        <v>45799.77083333334</v>
-      </c>
-      <c r="B268">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2">
-      <c r="A269" s="2">
-        <v>45799.78125</v>
-      </c>
-      <c r="B269">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2">
-      <c r="A270" s="2">
-        <v>45799.79166666666</v>
-      </c>
-      <c r="B270">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2">
-      <c r="A271" s="2">
-        <v>45799.80208333334</v>
-      </c>
-      <c r="B271">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2">
-      <c r="A272" s="2">
-        <v>45799.8125</v>
-      </c>
-      <c r="B272">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2">
-      <c r="A273" s="2">
-        <v>45799.82291666666</v>
-      </c>
-      <c r="B273">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2">
-      <c r="A274" s="2">
-        <v>45799.83333333334</v>
-      </c>
-      <c r="B274">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2">
-      <c r="A275" s="2">
-        <v>45799.84375</v>
-      </c>
-      <c r="B275">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2">
-      <c r="A276" s="2">
-        <v>45799.85416666666</v>
-      </c>
-      <c r="B276">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2">
-      <c r="A277" s="2">
-        <v>45799.86458333334</v>
-      </c>
-      <c r="B277">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2">
-      <c r="A278" s="2">
-        <v>45799.875</v>
-      </c>
-      <c r="B278">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2">
-      <c r="A279" s="2">
-        <v>45799.88541666666</v>
-      </c>
-      <c r="B279">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2">
-      <c r="A280" s="2">
-        <v>45799.89583333334</v>
-      </c>
-      <c r="B280">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2">
-      <c r="A281" s="2">
-        <v>45799.90625</v>
-      </c>
-      <c r="B281">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2">
-      <c r="A282" s="2">
-        <v>45799.91666666666</v>
-      </c>
-      <c r="B282">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2">
-      <c r="A283" s="2">
-        <v>45799.92708333334</v>
-      </c>
-      <c r="B283">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2">
-      <c r="A284" s="2">
-        <v>45799.9375</v>
-      </c>
-      <c r="B284">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2">
-      <c r="A285" s="2">
-        <v>45799.94791666666</v>
-      </c>
-      <c r="B285">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2">
-      <c r="A286" s="2">
-        <v>45799.95833333334</v>
-      </c>
-      <c r="B286">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2">
-      <c r="A287" s="2">
-        <v>45799.96875</v>
-      </c>
-      <c r="B287">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2">
-      <c r="A288" s="2">
-        <v>45799.97916666666</v>
-      </c>
-      <c r="B288">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2">
-      <c r="A289" s="2">
-        <v>45799.98958333334</v>
-      </c>
-      <c r="B289">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Retraining the models for GESS
</commit_message>
<xml_diff>
--- a/data_fetching/Entsoe/Actual_Production_Hydro_River.xlsx
+++ b/data_fetching/Entsoe/Actual_Production_Hydro_River.xlsx
@@ -397,127 +397,127 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="B2">
-        <v>576</v>
+        <v>625</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>46047.01041666666</v>
+        <v>46048.01041666666</v>
       </c>
       <c r="B3">
-        <v>570</v>
+        <v>579</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>46047.02083333334</v>
+        <v>46048.02083333334</v>
       </c>
       <c r="B4">
-        <v>600</v>
+        <v>578</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>46047.03125</v>
+        <v>46048.03125</v>
       </c>
       <c r="B5">
-        <v>601</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>46047.04166666666</v>
+        <v>46048.04166666666</v>
       </c>
       <c r="B6">
-        <v>576</v>
+        <v>564</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>46047.05208333334</v>
+        <v>46048.05208333334</v>
       </c>
       <c r="B7">
-        <v>571</v>
+        <v>563</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>46047.0625</v>
+        <v>46048.0625</v>
       </c>
       <c r="B8">
-        <v>572</v>
+        <v>564</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>46047.07291666666</v>
+        <v>46048.07291666666</v>
       </c>
       <c r="B9">
-        <v>571</v>
+        <v>563</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>46047.08333333334</v>
+        <v>46048.08333333334</v>
       </c>
       <c r="B10">
-        <v>572</v>
+        <v>560</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>46047.09375</v>
+        <v>46048.09375</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>558</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>46047.10416666666</v>
+        <v>46048.10416666666</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>559</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>46047.11458333334</v>
+        <v>46048.11458333334</v>
       </c>
       <c r="B13">
-        <v>571</v>
+        <v>558</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>46047.125</v>
+        <v>46048.125</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>553</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>46047.13541666666</v>
+        <v>46048.13541666666</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>530</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>46047.14583333334</v>
+        <v>46048.14583333334</v>
       </c>
       <c r="B16">
-        <v>572</v>
+        <v>529</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>46047.15625</v>
+        <v>46048.15625</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -525,479 +525,479 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>46047.16666666666</v>
+        <v>46048.16666666666</v>
       </c>
       <c r="B18">
-        <v>589</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>46047.17708333334</v>
+        <v>46048.17708333334</v>
       </c>
       <c r="B19">
-        <v>591</v>
+        <v>536</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>46047.1875</v>
+        <v>46048.1875</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>535</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>46047.19791666666</v>
+        <v>46048.19791666666</v>
       </c>
       <c r="B21">
-        <v>592</v>
+        <v>537</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>46047.20833333334</v>
+        <v>46048.20833333334</v>
       </c>
       <c r="B22">
-        <v>635</v>
+        <v>573</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>46047.21875</v>
+        <v>46048.21875</v>
       </c>
       <c r="B23">
-        <v>637</v>
+        <v>590</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>46047.22916666666</v>
+        <v>46048.22916666666</v>
       </c>
       <c r="B24">
-        <v>669</v>
+        <v>596</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>46047.23958333334</v>
+        <v>46048.23958333334</v>
       </c>
       <c r="B25">
-        <v>672</v>
+        <v>615</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>46047.25</v>
+        <v>46048.25</v>
       </c>
       <c r="B26">
-        <v>613</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
-        <v>46047.26041666666</v>
+        <v>46048.26041666666</v>
       </c>
       <c r="B27">
-        <v>612</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
-        <v>46047.27083333334</v>
+        <v>46048.27083333334</v>
       </c>
       <c r="B28">
-        <v>613</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
-        <v>46047.28125</v>
+        <v>46048.28125</v>
       </c>
       <c r="B29">
-        <v>656</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2">
-        <v>46047.29166666666</v>
+        <v>46048.29166666666</v>
       </c>
       <c r="B30">
-        <v>1141</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2">
-        <v>46047.30208333334</v>
+        <v>46048.30208333334</v>
       </c>
       <c r="B31">
-        <v>1150</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2">
-        <v>46047.3125</v>
+        <v>46048.3125</v>
       </c>
       <c r="B32">
-        <v>1155</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2">
-        <v>46047.32291666666</v>
+        <v>46048.32291666666</v>
       </c>
       <c r="B33">
-        <v>1177</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2">
-        <v>46047.33333333334</v>
+        <v>46048.33333333334</v>
       </c>
       <c r="B34">
-        <v>1303</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2">
-        <v>46047.34375</v>
+        <v>46048.34375</v>
       </c>
       <c r="B35">
-        <v>1312</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2">
-        <v>46047.35416666666</v>
+        <v>46048.35416666666</v>
       </c>
       <c r="B36">
-        <v>1316</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2">
-        <v>46047.36458333334</v>
+        <v>46048.36458333334</v>
       </c>
       <c r="B37">
-        <v>1286</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2">
-        <v>46047.375</v>
+        <v>46048.375</v>
       </c>
       <c r="B38">
-        <v>1300</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2">
-        <v>46047.38541666666</v>
+        <v>46048.38541666666</v>
       </c>
       <c r="B39">
-        <v>1302</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2">
-        <v>46047.39583333334</v>
+        <v>46048.39583333334</v>
       </c>
       <c r="B40">
-        <v>1295</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2">
-        <v>46047.40625</v>
+        <v>46048.40625</v>
       </c>
       <c r="B41">
-        <v>1302</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2">
-        <v>46047.41666666666</v>
+        <v>46048.41666666666</v>
       </c>
       <c r="B42">
-        <v>1297</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2">
-        <v>46047.42708333334</v>
+        <v>46048.42708333334</v>
       </c>
       <c r="B43">
-        <v>1295</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2">
-        <v>46047.4375</v>
+        <v>46048.4375</v>
       </c>
       <c r="B44">
-        <v>1297</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2">
-        <v>46047.44791666666</v>
+        <v>46048.44791666666</v>
       </c>
       <c r="B45">
-        <v>1295</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2">
-        <v>46047.45833333334</v>
+        <v>46048.45833333334</v>
       </c>
       <c r="B46">
-        <v>1306</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2">
-        <v>46047.46875</v>
+        <v>46048.46875</v>
       </c>
       <c r="B47">
-        <v>1303</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2">
-        <v>46047.47916666666</v>
+        <v>46048.47916666666</v>
       </c>
       <c r="B48">
-        <v>1305</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2">
-        <v>46047.48958333334</v>
+        <v>46048.48958333334</v>
       </c>
       <c r="B49">
-        <v>1302</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2">
-        <v>46047.5</v>
+        <v>46048.5</v>
       </c>
       <c r="B50">
-        <v>1014</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2">
-        <v>46047.51041666666</v>
+        <v>46048.51041666666</v>
       </c>
       <c r="B51">
-        <v>1004</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2">
-        <v>46047.52083333334</v>
+        <v>46048.52083333334</v>
       </c>
       <c r="B52">
-        <v>1005</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2">
-        <v>46047.53125</v>
+        <v>46048.53125</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2">
-        <v>46047.54166666666</v>
+        <v>46048.54166666666</v>
       </c>
       <c r="B54">
-        <v>961</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2">
-        <v>46047.55208333334</v>
+        <v>46048.55208333334</v>
       </c>
       <c r="B55">
-        <v>963</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2">
-        <v>46047.5625</v>
+        <v>46048.5625</v>
       </c>
       <c r="B56">
-        <v>967</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2">
-        <v>46047.57291666666</v>
+        <v>46048.57291666666</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>996</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2">
-        <v>46047.58333333334</v>
+        <v>46048.58333333334</v>
       </c>
       <c r="B58">
-        <v>1014</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2">
-        <v>46047.59375</v>
+        <v>46048.59375</v>
       </c>
       <c r="B59">
-        <v>1016</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2">
-        <v>46047.60416666666</v>
+        <v>46048.60416666666</v>
       </c>
       <c r="B60">
-        <v>1008</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2">
-        <v>46047.61458333334</v>
+        <v>46048.61458333334</v>
       </c>
       <c r="B61">
-        <v>1016</v>
+        <v>952</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2">
-        <v>46047.625</v>
+        <v>46048.625</v>
       </c>
       <c r="B62">
-        <v>1225</v>
+        <v>971</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2">
-        <v>46047.63541666666</v>
+        <v>46048.63541666666</v>
       </c>
       <c r="B63">
-        <v>1228</v>
+        <v>972</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2">
-        <v>46047.64583333334</v>
+        <v>46048.64583333334</v>
       </c>
       <c r="B64">
-        <v>1194</v>
+        <v>991</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2">
-        <v>46047.65625</v>
+        <v>46048.65625</v>
       </c>
       <c r="B65">
-        <v>1197</v>
+        <v>999</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2">
-        <v>46047.66666666666</v>
+        <v>46048.66666666666</v>
       </c>
       <c r="B66">
-        <v>1317</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2">
-        <v>46047.67708333334</v>
+        <v>46048.67708333334</v>
       </c>
       <c r="B67">
-        <v>1327</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2">
-        <v>46047.6875</v>
+        <v>46048.6875</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2">
-        <v>46047.69791666666</v>
+        <v>46048.69791666666</v>
       </c>
       <c r="B69">
-        <v>1320</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2">
-        <v>46047.70833333334</v>
+        <v>46048.70833333334</v>
       </c>
       <c r="B70">
-        <v>1342</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2">
-        <v>46047.71875</v>
+        <v>46048.71875</v>
       </c>
       <c r="B71">
-        <v>1346</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="2">
-        <v>46047.72916666666</v>
+        <v>46048.72916666666</v>
       </c>
       <c r="B72">
-        <v>1345</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2">
-        <v>46047.73958333334</v>
+        <v>46048.73958333334</v>
       </c>
       <c r="B73">
-        <v>1347</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="2">
-        <v>46047.75</v>
+        <v>46048.75</v>
       </c>
       <c r="B74">
-        <v>1369</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="2">
-        <v>46047.76041666666</v>
+        <v>46048.76041666666</v>
       </c>
       <c r="B75">
-        <v>1373</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="2">
-        <v>46047.77083333334</v>
+        <v>46048.77083333334</v>
       </c>
       <c r="B76">
-        <v>1396</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="2">
-        <v>46047.78125</v>
+        <v>46048.78125</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -1005,415 +1005,415 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="2">
-        <v>46047.79166666666</v>
+        <v>46048.79166666666</v>
       </c>
       <c r="B78">
-        <v>1377</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="2">
-        <v>46047.80208333334</v>
+        <v>46048.80208333334</v>
       </c>
       <c r="B79">
-        <v>1371</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="2">
-        <v>46047.8125</v>
+        <v>46048.8125</v>
       </c>
       <c r="B80">
-        <v>1334</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="2">
-        <v>46047.82291666666</v>
+        <v>46048.82291666666</v>
       </c>
       <c r="B81">
-        <v>1332</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="2">
-        <v>46047.83333333334</v>
+        <v>46048.83333333334</v>
       </c>
       <c r="B82">
-        <v>1327</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="2">
-        <v>46047.84375</v>
+        <v>46048.84375</v>
       </c>
       <c r="B83">
-        <v>1325</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="2">
-        <v>46047.85416666666</v>
+        <v>46048.85416666666</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="2">
-        <v>46047.86458333334</v>
+        <v>46048.86458333334</v>
       </c>
       <c r="B85">
-        <v>1301</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="2">
-        <v>46047.875</v>
+        <v>46048.875</v>
       </c>
       <c r="B86">
-        <v>1025</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="2">
-        <v>46047.88541666666</v>
+        <v>46048.88541666666</v>
       </c>
       <c r="B87">
-        <v>898</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="2">
-        <v>46047.89583333334</v>
+        <v>46048.89583333334</v>
       </c>
       <c r="B88">
-        <v>950</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="2">
-        <v>46047.90625</v>
+        <v>46048.90625</v>
       </c>
       <c r="B89">
-        <v>953</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="2">
-        <v>46047.91666666666</v>
+        <v>46048.91666666666</v>
       </c>
       <c r="B90">
-        <v>800</v>
+        <v>885</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="2">
-        <v>46047.92708333334</v>
+        <v>46048.92708333334</v>
       </c>
       <c r="B91">
-        <v>795</v>
+        <v>859</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="2">
-        <v>46047.9375</v>
+        <v>46048.9375</v>
       </c>
       <c r="B92">
-        <v>827</v>
+        <v>861</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="2">
-        <v>46047.94791666666</v>
+        <v>46048.94791666666</v>
       </c>
       <c r="B93">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="2">
-        <v>46047.95833333334</v>
+        <v>46048.95833333334</v>
       </c>
       <c r="B94">
-        <v>686</v>
+        <v>669</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="2">
-        <v>46047.96875</v>
+        <v>46048.96875</v>
       </c>
       <c r="B95">
-        <v>674</v>
+        <v>648</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="2">
-        <v>46047.97916666666</v>
+        <v>46048.97916666666</v>
       </c>
       <c r="B96">
-        <v>677</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="2">
-        <v>46047.98958333334</v>
+        <v>46048.98958333334</v>
       </c>
       <c r="B97">
-        <v>674</v>
+        <v>645</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="2">
-        <v>46048</v>
+        <v>46049</v>
       </c>
       <c r="B98">
-        <v>625</v>
+        <v>593</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="2">
-        <v>46048.01041666666</v>
+        <v>46049.01041666666</v>
       </c>
       <c r="B99">
-        <v>579</v>
+        <v>522</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="2">
-        <v>46048.02083333334</v>
+        <v>46049.02083333334</v>
       </c>
       <c r="B100">
-        <v>578</v>
+        <v>603</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="2">
-        <v>46048.03125</v>
+        <v>46049.03125</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>616</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="2">
-        <v>46048.04166666666</v>
+        <v>46049.04166666666</v>
       </c>
       <c r="B102">
-        <v>564</v>
+        <v>584</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="2">
-        <v>46048.05208333334</v>
+        <v>46049.05208333334</v>
       </c>
       <c r="B103">
-        <v>563</v>
+        <v>581</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="2">
-        <v>46048.0625</v>
+        <v>46049.0625</v>
       </c>
       <c r="B104">
-        <v>564</v>
+        <v>586</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="2">
-        <v>46048.07291666666</v>
+        <v>46049.07291666666</v>
       </c>
       <c r="B105">
-        <v>563</v>
+        <v>584</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="2">
-        <v>46048.08333333334</v>
+        <v>46049.08333333334</v>
       </c>
       <c r="B106">
-        <v>560</v>
+        <v>586</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="2">
-        <v>46048.09375</v>
+        <v>46049.09375</v>
       </c>
       <c r="B107">
-        <v>558</v>
+        <v>585</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="2">
-        <v>46048.10416666666</v>
+        <v>46049.10416666666</v>
       </c>
       <c r="B108">
-        <v>559</v>
+        <v>472</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="2">
-        <v>46048.11458333334</v>
+        <v>46049.11458333334</v>
       </c>
       <c r="B109">
-        <v>558</v>
+        <v>438</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="2">
-        <v>46048.125</v>
+        <v>46049.125</v>
       </c>
       <c r="B110">
-        <v>553</v>
+        <v>450</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="2">
-        <v>46048.13541666666</v>
+        <v>46049.13541666666</v>
       </c>
       <c r="B111">
-        <v>530</v>
+        <v>452</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="2">
-        <v>46048.14583333334</v>
+        <v>46049.14583333334</v>
       </c>
       <c r="B112">
-        <v>529</v>
+        <v>588</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="2">
-        <v>46048.15625</v>
+        <v>46049.15625</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>665</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="2">
-        <v>46048.16666666666</v>
+        <v>46049.16666666666</v>
       </c>
       <c r="B114">
-        <v>0</v>
+        <v>723</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="2">
-        <v>46048.17708333334</v>
+        <v>46049.17708333334</v>
       </c>
       <c r="B115">
-        <v>536</v>
+        <v>732</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="2">
-        <v>46048.1875</v>
+        <v>46049.1875</v>
       </c>
       <c r="B116">
-        <v>535</v>
+        <v>735</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="2">
-        <v>46048.19791666666</v>
+        <v>46049.19791666666</v>
       </c>
       <c r="B117">
-        <v>537</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="2">
-        <v>46048.20833333334</v>
+        <v>46049.20833333334</v>
       </c>
       <c r="B118">
-        <v>573</v>
+        <v>691</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="2">
-        <v>46048.21875</v>
+        <v>46049.21875</v>
       </c>
       <c r="B119">
-        <v>590</v>
+        <v>690</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="2">
-        <v>46048.22916666666</v>
+        <v>46049.22916666666</v>
       </c>
       <c r="B120">
-        <v>596</v>
+        <v>685</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="2">
-        <v>46048.23958333334</v>
+        <v>46049.23958333334</v>
       </c>
       <c r="B121">
-        <v>615</v>
+        <v>694</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="2">
-        <v>46048.25</v>
+        <v>46049.25</v>
       </c>
       <c r="B122">
-        <v>1024</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="2">
-        <v>46048.26041666666</v>
+        <v>46049.26041666666</v>
       </c>
       <c r="B123">
-        <v>1076</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="2">
-        <v>46048.27083333334</v>
+        <v>46049.27083333334</v>
       </c>
       <c r="B124">
-        <v>1123</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="2">
-        <v>46048.28125</v>
+        <v>46049.28125</v>
       </c>
       <c r="B125">
-        <v>1134</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="2">
-        <v>46048.29166666666</v>
+        <v>46049.29166666666</v>
       </c>
       <c r="B126">
-        <v>1260</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="2">
-        <v>46048.30208333334</v>
+        <v>46049.30208333334</v>
       </c>
       <c r="B127">
-        <v>1174</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="2">
-        <v>46048.3125</v>
+        <v>46049.3125</v>
       </c>
       <c r="B128">
-        <v>1159</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="2">
-        <v>46048.32291666666</v>
+        <v>46049.32291666666</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -1421,95 +1421,95 @@
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="2">
-        <v>46048.33333333334</v>
+        <v>46049.33333333334</v>
       </c>
       <c r="B130">
-        <v>1169</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="2">
-        <v>46048.34375</v>
+        <v>46049.34375</v>
       </c>
       <c r="B131">
-        <v>1166</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="2">
-        <v>46048.35416666666</v>
+        <v>46049.35416666666</v>
       </c>
       <c r="B132">
-        <v>0</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="2">
-        <v>46048.36458333334</v>
+        <v>46049.36458333334</v>
       </c>
       <c r="B133">
-        <v>1167</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="2">
-        <v>46048.375</v>
+        <v>46049.375</v>
       </c>
       <c r="B134">
-        <v>1137</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="2">
-        <v>46048.38541666666</v>
+        <v>46049.38541666666</v>
       </c>
       <c r="B135">
-        <v>1193</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="2">
-        <v>46048.39583333334</v>
+        <v>46049.39583333334</v>
       </c>
       <c r="B136">
-        <v>1210</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="2">
-        <v>46048.40625</v>
+        <v>46049.40625</v>
       </c>
       <c r="B137">
-        <v>1249</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="2">
-        <v>46048.41666666666</v>
+        <v>46049.41666666666</v>
       </c>
       <c r="B138">
-        <v>1236</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="2">
-        <v>46048.42708333334</v>
+        <v>46049.42708333334</v>
       </c>
       <c r="B139">
-        <v>1234</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="2">
-        <v>46048.4375</v>
+        <v>46049.4375</v>
       </c>
       <c r="B140">
-        <v>0</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="2">
-        <v>46048.44791666666</v>
+        <v>46049.44791666666</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="2">
-        <v>46048.45833333334</v>
+        <v>46049.45833333334</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="2">
-        <v>46048.46875</v>
+        <v>46049.46875</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="2">
-        <v>46048.47916666666</v>
+        <v>46049.47916666666</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="2">
-        <v>46048.48958333334</v>
+        <v>46049.48958333334</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="2">
-        <v>46048.5</v>
+        <v>46049.5</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="2">
-        <v>46048.51041666666</v>
+        <v>46049.51041666666</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2">
-        <v>46048.52083333334</v>
+        <v>46049.52083333334</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="2">
-        <v>46048.53125</v>
+        <v>46049.53125</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="2">
-        <v>46048.54166666666</v>
+        <v>46049.54166666666</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -1589,7 +1589,7 @@
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="2">
-        <v>46048.55208333334</v>
+        <v>46049.55208333334</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="2">
-        <v>46048.5625</v>
+        <v>46049.5625</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -1605,7 +1605,7 @@
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="2">
-        <v>46048.57291666666</v>
+        <v>46049.57291666666</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -1613,7 +1613,7 @@
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="2">
-        <v>46048.58333333334</v>
+        <v>46049.58333333334</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -1621,7 +1621,7 @@
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="2">
-        <v>46048.59375</v>
+        <v>46049.59375</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -1629,7 +1629,7 @@
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="2">
-        <v>46048.60416666666</v>
+        <v>46049.60416666666</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="2">
-        <v>46048.61458333334</v>
+        <v>46049.61458333334</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -1645,7 +1645,7 @@
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="2">
-        <v>46048.625</v>
+        <v>46049.625</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -1653,7 +1653,7 @@
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="2">
-        <v>46048.63541666666</v>
+        <v>46049.63541666666</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -1661,7 +1661,7 @@
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="2">
-        <v>46048.64583333334</v>
+        <v>46049.64583333334</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -1669,7 +1669,7 @@
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="2">
-        <v>46048.65625</v>
+        <v>46049.65625</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="2">
-        <v>46048.66666666666</v>
+        <v>46049.66666666666</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="2">
-        <v>46048.67708333334</v>
+        <v>46049.67708333334</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -1693,7 +1693,7 @@
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="2">
-        <v>46048.6875</v>
+        <v>46049.6875</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -1701,7 +1701,7 @@
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="2">
-        <v>46048.69791666666</v>
+        <v>46049.69791666666</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -1709,7 +1709,7 @@
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="2">
-        <v>46048.70833333334</v>
+        <v>46049.70833333334</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -1717,7 +1717,7 @@
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="2">
-        <v>46048.71875</v>
+        <v>46049.71875</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="2">
-        <v>46048.72916666666</v>
+        <v>46049.72916666666</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="2">
-        <v>46048.73958333334</v>
+        <v>46049.73958333334</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -1741,7 +1741,7 @@
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="2">
-        <v>46048.75</v>
+        <v>46049.75</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -1749,7 +1749,7 @@
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="2">
-        <v>46048.76041666666</v>
+        <v>46049.76041666666</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -1757,7 +1757,7 @@
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="2">
-        <v>46048.77083333334</v>
+        <v>46049.77083333334</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -1765,7 +1765,7 @@
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="2">
-        <v>46048.78125</v>
+        <v>46049.78125</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -1773,7 +1773,7 @@
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="2">
-        <v>46048.79166666666</v>
+        <v>46049.79166666666</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="2">
-        <v>46048.80208333334</v>
+        <v>46049.80208333334</v>
       </c>
       <c r="B175">
         <v>0</v>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="2">
-        <v>46048.8125</v>
+        <v>46049.8125</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="177" spans="1:2">
       <c r="A177" s="2">
-        <v>46048.82291666666</v>
+        <v>46049.82291666666</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -1805,7 +1805,7 @@
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="2">
-        <v>46048.83333333334</v>
+        <v>46049.83333333334</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="179" spans="1:2">
       <c r="A179" s="2">
-        <v>46048.84375</v>
+        <v>46049.84375</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -1821,7 +1821,7 @@
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="2">
-        <v>46048.85416666666</v>
+        <v>46049.85416666666</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="2">
-        <v>46048.86458333334</v>
+        <v>46049.86458333334</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -1837,7 +1837,7 @@
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="2">
-        <v>46048.875</v>
+        <v>46049.875</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -1845,7 +1845,7 @@
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="2">
-        <v>46048.88541666666</v>
+        <v>46049.88541666666</v>
       </c>
       <c r="B183">
         <v>0</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="2">
-        <v>46048.89583333334</v>
+        <v>46049.89583333334</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -1861,7 +1861,7 @@
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="2">
-        <v>46048.90625</v>
+        <v>46049.90625</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -1869,7 +1869,7 @@
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="2">
-        <v>46048.91666666666</v>
+        <v>46049.91666666666</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="2">
-        <v>46048.92708333334</v>
+        <v>46049.92708333334</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="188" spans="1:2">
       <c r="A188" s="2">
-        <v>46048.9375</v>
+        <v>46049.9375</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -1893,7 +1893,7 @@
     </row>
     <row r="189" spans="1:2">
       <c r="A189" s="2">
-        <v>46048.94791666666</v>
+        <v>46049.94791666666</v>
       </c>
       <c r="B189">
         <v>0</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="2">
-        <v>46048.95833333334</v>
+        <v>46049.95833333334</v>
       </c>
       <c r="B190">
         <v>0</v>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="191" spans="1:2">
       <c r="A191" s="2">
-        <v>46048.96875</v>
+        <v>46049.96875</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="2">
-        <v>46048.97916666666</v>
+        <v>46049.97916666666</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -1925,7 +1925,7 @@
     </row>
     <row r="193" spans="1:2">
       <c r="A193" s="2">
-        <v>46048.98958333334</v>
+        <v>46049.98958333334</v>
       </c>
       <c r="B193">
         <v>0</v>

</xml_diff>